<commit_message>
no transkip D3 Kep
</commit_message>
<xml_diff>
--- a/D3 Keperawatan/Transkip Nilai D3 Kep.xlsx
+++ b/D3 Keperawatan/Transkip Nilai D3 Kep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\D3 Keperawatan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54314616-1173-4069-9E06-AB8405D25972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D2958CE-AD1C-4831-AF1C-441209326C5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22668FF5-9BBF-4EB6-990E-3DE3502F0C5B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2259" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2300" uniqueCount="269">
   <si>
     <t>NO</t>
   </si>
@@ -719,6 +719,129 @@
   <si>
     <t>Implementasi Latihan Keseimbangan Pada Lanjut Usia Di Rumah Bahagia Embung Fatimah Kota Tanjung Pinang</t>
   </si>
+  <si>
+    <t>953 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>954 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>955 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>956 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>957 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>958 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>959 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>960 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>961 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>962 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>963 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>964 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>965 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>966 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>967 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>968 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>969 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>970 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>971 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>972 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>973 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>974 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>975 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>976 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>977 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>978 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>979 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>980 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>981 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>982 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>983 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>984 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>985 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>986 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>987 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>988 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>989 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>990 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>991 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>992 / 13 / XII / 2025</t>
+  </si>
+  <si>
+    <t>993 / 13 / XII / 2025</t>
+  </si>
 </sst>
 </file>
 
@@ -727,7 +850,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -784,8 +907,21 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -846,6 +982,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -871,13 +1012,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -937,33 +1079,6 @@
     <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -973,8 +1088,39 @@
     <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Good 2" xfId="4" xr:uid="{9E58217C-29C0-4F6B-BCCA-FBD9D11D267D}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2 2" xfId="3" xr:uid="{1A2E649E-1D69-49E3-9F85-E51B2FE11459}"/>
     <cellStyle name="Normal 4" xfId="1" xr:uid="{503719C2-763D-4B57-94FE-6D2DAEA00D00}"/>
@@ -1293,10 +1439,10 @@
   <dimension ref="A1:IJ44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="II15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
+      <selection pane="bottomRight" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1314,22 +1460,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:244" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="32" t="s">
+      <c r="C1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="E1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="28" t="s">
         <v>43</v>
       </c>
       <c r="G1" s="31" t="s">
@@ -1451,257 +1597,257 @@
       <c r="CK1" s="30"/>
       <c r="CL1" s="30"/>
       <c r="CM1" s="30"/>
-      <c r="CN1" s="29" t="s">
+      <c r="CN1" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="CO1" s="29"/>
-      <c r="CP1" s="29"/>
-      <c r="CQ1" s="29"/>
-      <c r="CR1" s="29"/>
-      <c r="CS1" s="29" t="s">
+      <c r="CO1" s="32"/>
+      <c r="CP1" s="32"/>
+      <c r="CQ1" s="32"/>
+      <c r="CR1" s="32"/>
+      <c r="CS1" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="CT1" s="29"/>
-      <c r="CU1" s="29"/>
-      <c r="CV1" s="29"/>
-      <c r="CW1" s="29"/>
-      <c r="CX1" s="29" t="s">
+      <c r="CT1" s="32"/>
+      <c r="CU1" s="32"/>
+      <c r="CV1" s="32"/>
+      <c r="CW1" s="32"/>
+      <c r="CX1" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="CY1" s="29"/>
-      <c r="CZ1" s="29"/>
-      <c r="DA1" s="29"/>
-      <c r="DB1" s="29"/>
-      <c r="DC1" s="29" t="s">
+      <c r="CY1" s="32"/>
+      <c r="CZ1" s="32"/>
+      <c r="DA1" s="32"/>
+      <c r="DB1" s="32"/>
+      <c r="DC1" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="DD1" s="29"/>
-      <c r="DE1" s="29"/>
-      <c r="DF1" s="29"/>
-      <c r="DG1" s="29"/>
-      <c r="DH1" s="29" t="s">
+      <c r="DD1" s="32"/>
+      <c r="DE1" s="32"/>
+      <c r="DF1" s="32"/>
+      <c r="DG1" s="32"/>
+      <c r="DH1" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="DI1" s="29"/>
-      <c r="DJ1" s="29"/>
-      <c r="DK1" s="29"/>
-      <c r="DL1" s="29"/>
-      <c r="DM1" s="29" t="s">
+      <c r="DI1" s="32"/>
+      <c r="DJ1" s="32"/>
+      <c r="DK1" s="32"/>
+      <c r="DL1" s="32"/>
+      <c r="DM1" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="DN1" s="29"/>
-      <c r="DO1" s="29"/>
-      <c r="DP1" s="29"/>
-      <c r="DQ1" s="29"/>
-      <c r="DR1" s="29" t="s">
+      <c r="DN1" s="32"/>
+      <c r="DO1" s="32"/>
+      <c r="DP1" s="32"/>
+      <c r="DQ1" s="32"/>
+      <c r="DR1" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="DS1" s="29"/>
-      <c r="DT1" s="29"/>
-      <c r="DU1" s="29"/>
-      <c r="DV1" s="29"/>
-      <c r="DW1" s="29" t="s">
+      <c r="DS1" s="32"/>
+      <c r="DT1" s="32"/>
+      <c r="DU1" s="32"/>
+      <c r="DV1" s="32"/>
+      <c r="DW1" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="DX1" s="29"/>
-      <c r="DY1" s="29"/>
-      <c r="DZ1" s="29"/>
-      <c r="EA1" s="29"/>
-      <c r="EB1" s="28" t="s">
+      <c r="DX1" s="32"/>
+      <c r="DY1" s="32"/>
+      <c r="DZ1" s="32"/>
+      <c r="EA1" s="32"/>
+      <c r="EB1" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="EC1" s="28"/>
-      <c r="ED1" s="28"/>
-      <c r="EE1" s="28"/>
-      <c r="EF1" s="28"/>
-      <c r="EG1" s="28" t="s">
+      <c r="EC1" s="34"/>
+      <c r="ED1" s="34"/>
+      <c r="EE1" s="34"/>
+      <c r="EF1" s="34"/>
+      <c r="EG1" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="EH1" s="28"/>
-      <c r="EI1" s="28"/>
-      <c r="EJ1" s="28"/>
-      <c r="EK1" s="28"/>
-      <c r="EL1" s="28" t="s">
+      <c r="EH1" s="34"/>
+      <c r="EI1" s="34"/>
+      <c r="EJ1" s="34"/>
+      <c r="EK1" s="34"/>
+      <c r="EL1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="EM1" s="28"/>
-      <c r="EN1" s="28"/>
-      <c r="EO1" s="28"/>
-      <c r="EP1" s="28"/>
-      <c r="EQ1" s="28" t="s">
+      <c r="EM1" s="34"/>
+      <c r="EN1" s="34"/>
+      <c r="EO1" s="34"/>
+      <c r="EP1" s="34"/>
+      <c r="EQ1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="ER1" s="28"/>
-      <c r="ES1" s="28"/>
-      <c r="ET1" s="28"/>
-      <c r="EU1" s="28"/>
-      <c r="EV1" s="28" t="s">
+      <c r="ER1" s="34"/>
+      <c r="ES1" s="34"/>
+      <c r="ET1" s="34"/>
+      <c r="EU1" s="34"/>
+      <c r="EV1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="EW1" s="28"/>
-      <c r="EX1" s="28"/>
-      <c r="EY1" s="28"/>
-      <c r="EZ1" s="28"/>
-      <c r="FA1" s="28" t="s">
+      <c r="EW1" s="34"/>
+      <c r="EX1" s="34"/>
+      <c r="EY1" s="34"/>
+      <c r="EZ1" s="34"/>
+      <c r="FA1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="FB1" s="28"/>
-      <c r="FC1" s="28"/>
-      <c r="FD1" s="28"/>
-      <c r="FE1" s="28"/>
-      <c r="FF1" s="28" t="s">
+      <c r="FB1" s="34"/>
+      <c r="FC1" s="34"/>
+      <c r="FD1" s="34"/>
+      <c r="FE1" s="34"/>
+      <c r="FF1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="FG1" s="28"/>
-      <c r="FH1" s="28"/>
-      <c r="FI1" s="28"/>
-      <c r="FJ1" s="28"/>
-      <c r="FK1" s="28" t="s">
+      <c r="FG1" s="34"/>
+      <c r="FH1" s="34"/>
+      <c r="FI1" s="34"/>
+      <c r="FJ1" s="34"/>
+      <c r="FK1" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="FL1" s="28"/>
-      <c r="FM1" s="28"/>
-      <c r="FN1" s="28"/>
-      <c r="FO1" s="28"/>
-      <c r="FP1" s="27" t="s">
+      <c r="FL1" s="34"/>
+      <c r="FM1" s="34"/>
+      <c r="FN1" s="34"/>
+      <c r="FO1" s="34"/>
+      <c r="FP1" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="FQ1" s="27"/>
-      <c r="FR1" s="27"/>
-      <c r="FS1" s="27"/>
-      <c r="FT1" s="27"/>
-      <c r="FU1" s="27" t="s">
+      <c r="FQ1" s="33"/>
+      <c r="FR1" s="33"/>
+      <c r="FS1" s="33"/>
+      <c r="FT1" s="33"/>
+      <c r="FU1" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="FV1" s="27"/>
-      <c r="FW1" s="27"/>
-      <c r="FX1" s="27"/>
-      <c r="FY1" s="27"/>
-      <c r="FZ1" s="27" t="s">
+      <c r="FV1" s="33"/>
+      <c r="FW1" s="33"/>
+      <c r="FX1" s="33"/>
+      <c r="FY1" s="33"/>
+      <c r="FZ1" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="GA1" s="27"/>
-      <c r="GB1" s="27"/>
-      <c r="GC1" s="27"/>
-      <c r="GD1" s="27"/>
-      <c r="GE1" s="27" t="s">
+      <c r="GA1" s="33"/>
+      <c r="GB1" s="33"/>
+      <c r="GC1" s="33"/>
+      <c r="GD1" s="33"/>
+      <c r="GE1" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="GF1" s="27"/>
-      <c r="GG1" s="27"/>
-      <c r="GH1" s="27"/>
-      <c r="GI1" s="27"/>
-      <c r="GJ1" s="27" t="s">
+      <c r="GF1" s="33"/>
+      <c r="GG1" s="33"/>
+      <c r="GH1" s="33"/>
+      <c r="GI1" s="33"/>
+      <c r="GJ1" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="GK1" s="27"/>
-      <c r="GL1" s="27"/>
-      <c r="GM1" s="27"/>
-      <c r="GN1" s="27"/>
-      <c r="GO1" s="27" t="s">
+      <c r="GK1" s="33"/>
+      <c r="GL1" s="33"/>
+      <c r="GM1" s="33"/>
+      <c r="GN1" s="33"/>
+      <c r="GO1" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="GP1" s="27"/>
-      <c r="GQ1" s="27"/>
-      <c r="GR1" s="27"/>
-      <c r="GS1" s="27"/>
-      <c r="GT1" s="27" t="s">
+      <c r="GP1" s="33"/>
+      <c r="GQ1" s="33"/>
+      <c r="GR1" s="33"/>
+      <c r="GS1" s="33"/>
+      <c r="GT1" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="GU1" s="27"/>
-      <c r="GV1" s="27"/>
-      <c r="GW1" s="27"/>
-      <c r="GX1" s="27"/>
-      <c r="GY1" s="27" t="s">
+      <c r="GU1" s="33"/>
+      <c r="GV1" s="33"/>
+      <c r="GW1" s="33"/>
+      <c r="GX1" s="33"/>
+      <c r="GY1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="GZ1" s="27"/>
-      <c r="HA1" s="27"/>
-      <c r="HB1" s="27"/>
-      <c r="HC1" s="27"/>
-      <c r="HD1" s="27" t="s">
+      <c r="GZ1" s="33"/>
+      <c r="HA1" s="33"/>
+      <c r="HB1" s="33"/>
+      <c r="HC1" s="33"/>
+      <c r="HD1" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="HE1" s="27"/>
-      <c r="HF1" s="27"/>
-      <c r="HG1" s="27"/>
-      <c r="HH1" s="27"/>
-      <c r="HI1" s="26" t="s">
+      <c r="HE1" s="33"/>
+      <c r="HF1" s="33"/>
+      <c r="HG1" s="33"/>
+      <c r="HH1" s="33"/>
+      <c r="HI1" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="HJ1" s="26"/>
-      <c r="HK1" s="26"/>
-      <c r="HL1" s="26"/>
-      <c r="HM1" s="26"/>
-      <c r="HN1" s="26" t="s">
+      <c r="HJ1" s="35"/>
+      <c r="HK1" s="35"/>
+      <c r="HL1" s="35"/>
+      <c r="HM1" s="35"/>
+      <c r="HN1" s="35" t="s">
         <v>166</v>
       </c>
-      <c r="HO1" s="26"/>
-      <c r="HP1" s="26"/>
-      <c r="HQ1" s="26"/>
-      <c r="HR1" s="26"/>
-      <c r="HS1" s="25" t="s">
+      <c r="HO1" s="35"/>
+      <c r="HP1" s="35"/>
+      <c r="HQ1" s="35"/>
+      <c r="HR1" s="35"/>
+      <c r="HS1" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="HT1" s="25" t="s">
+      <c r="HT1" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="HU1" s="25" t="s">
+      <c r="HU1" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="HV1" s="25" t="s">
+      <c r="HV1" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="HW1" s="25" t="s">
+      <c r="HW1" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="HX1" s="25" t="s">
+      <c r="HX1" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="HY1" s="25" t="s">
+      <c r="HY1" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="HZ1" s="25" t="s">
+      <c r="HZ1" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="IA1" s="25" t="s">
+      <c r="IA1" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="IB1" s="25" t="s">
+      <c r="IB1" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="IC1" s="25" t="s">
+      <c r="IC1" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="ID1" s="25" t="s">
+      <c r="ID1" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="IE1" s="25" t="s">
+      <c r="IE1" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="IF1" s="25" t="s">
+      <c r="IF1" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="IG1" s="25" t="s">
+      <c r="IG1" s="36" t="s">
         <v>190</v>
       </c>
-      <c r="IH1" s="25" t="s">
+      <c r="IH1" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="II1" s="25" t="s">
+      <c r="II1" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="IJ1" s="25" t="s">
+      <c r="IJ1" s="36" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:244" x14ac:dyDescent="0.25">
-      <c r="A2" s="32"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="32"/>
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="10" t="s">
         <v>44</v>
       </c>
@@ -2362,24 +2508,24 @@
       <c r="HR2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="HS2" s="25"/>
-      <c r="HT2" s="25"/>
-      <c r="HU2" s="25"/>
-      <c r="HV2" s="25"/>
-      <c r="HW2" s="25"/>
-      <c r="HX2" s="25"/>
-      <c r="HY2" s="25"/>
-      <c r="HZ2" s="25"/>
-      <c r="IA2" s="25"/>
-      <c r="IB2" s="25"/>
-      <c r="IC2" s="25"/>
-      <c r="ID2" s="25"/>
-      <c r="IE2" s="25"/>
-      <c r="IF2" s="25"/>
-      <c r="IG2" s="25"/>
-      <c r="IH2" s="25"/>
-      <c r="II2" s="25"/>
-      <c r="IJ2" s="25"/>
+      <c r="HS2" s="36"/>
+      <c r="HT2" s="36"/>
+      <c r="HU2" s="36"/>
+      <c r="HV2" s="36"/>
+      <c r="HW2" s="36"/>
+      <c r="HX2" s="36"/>
+      <c r="HY2" s="36"/>
+      <c r="HZ2" s="36"/>
+      <c r="IA2" s="36"/>
+      <c r="IB2" s="36"/>
+      <c r="IC2" s="36"/>
+      <c r="ID2" s="36"/>
+      <c r="IE2" s="36"/>
+      <c r="IF2" s="36"/>
+      <c r="IG2" s="36"/>
+      <c r="IH2" s="36"/>
+      <c r="II2" s="36"/>
+      <c r="IJ2" s="36"/>
     </row>
     <row r="3" spans="1:244" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
@@ -2397,7 +2543,9 @@
       <c r="E3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="6"/>
+      <c r="F3" s="37" t="s">
+        <v>228</v>
+      </c>
       <c r="G3" s="14">
         <v>87.6</v>
       </c>
@@ -3146,7 +3294,9 @@
       <c r="E4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="6"/>
+      <c r="F4" s="37" t="s">
+        <v>229</v>
+      </c>
       <c r="G4" s="14">
         <v>84.6</v>
       </c>
@@ -3895,7 +4045,9 @@
       <c r="E5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="6"/>
+      <c r="F5" s="37" t="s">
+        <v>230</v>
+      </c>
       <c r="G5" s="14">
         <v>85.35</v>
       </c>
@@ -4644,7 +4796,9 @@
       <c r="E6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="6"/>
+      <c r="F6" s="37" t="s">
+        <v>231</v>
+      </c>
       <c r="G6" s="14">
         <v>86.15</v>
       </c>
@@ -5393,7 +5547,9 @@
       <c r="E7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="6"/>
+      <c r="F7" s="37" t="s">
+        <v>232</v>
+      </c>
       <c r="G7" s="14">
         <v>86.95</v>
       </c>
@@ -6142,7 +6298,9 @@
       <c r="E8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="6"/>
+      <c r="F8" s="37" t="s">
+        <v>233</v>
+      </c>
       <c r="G8" s="14">
         <v>82.3</v>
       </c>
@@ -6879,7 +7037,7 @@
       <c r="A9" s="11">
         <v>7</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="26" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="8">
@@ -6891,7 +7049,9 @@
       <c r="E9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="6"/>
+      <c r="F9" s="37" t="s">
+        <v>234</v>
+      </c>
       <c r="G9" s="14">
         <v>84.1</v>
       </c>
@@ -7638,7 +7798,9 @@
       <c r="E10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="37" t="s">
+        <v>235</v>
+      </c>
       <c r="G10" s="14">
         <v>82.6</v>
       </c>
@@ -8387,7 +8549,9 @@
       <c r="E11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="37" t="s">
+        <v>236</v>
+      </c>
       <c r="G11" s="14">
         <v>79</v>
       </c>
@@ -9136,7 +9300,9 @@
       <c r="E12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="37" t="s">
+        <v>237</v>
+      </c>
       <c r="G12" s="14">
         <v>86.450000000000017</v>
       </c>
@@ -9885,7 +10051,9 @@
       <c r="E13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="37" t="s">
+        <v>238</v>
+      </c>
       <c r="G13" s="14">
         <v>91.35</v>
       </c>
@@ -10634,7 +10802,9 @@
       <c r="E14" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="37" t="s">
+        <v>239</v>
+      </c>
       <c r="G14" s="14">
         <v>88.1</v>
       </c>
@@ -11383,7 +11553,9 @@
       <c r="E15" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F15" s="6"/>
+      <c r="F15" s="37" t="s">
+        <v>240</v>
+      </c>
       <c r="G15" s="14">
         <v>85</v>
       </c>
@@ -12132,7 +12304,9 @@
       <c r="E16" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="F16" s="6"/>
+      <c r="F16" s="37" t="s">
+        <v>241</v>
+      </c>
       <c r="G16" s="14">
         <v>86.05</v>
       </c>
@@ -12861,7 +13035,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ16" s="34" t="s">
+      <c r="IJ16" s="25" t="s">
         <v>203</v>
       </c>
     </row>
@@ -12881,7 +13055,9 @@
       <c r="E17" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="F17" s="6"/>
+      <c r="F17" s="37" t="s">
+        <v>242</v>
+      </c>
       <c r="G17" s="14">
         <v>85.6</v>
       </c>
@@ -13630,7 +13806,9 @@
       <c r="E18" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="37" t="s">
+        <v>243</v>
+      </c>
       <c r="G18" s="14">
         <v>87.6</v>
       </c>
@@ -14379,7 +14557,9 @@
       <c r="E19" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="6"/>
+      <c r="F19" s="37" t="s">
+        <v>244</v>
+      </c>
       <c r="G19" s="14">
         <v>88.85</v>
       </c>
@@ -15128,7 +15308,9 @@
       <c r="E20" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="F20" s="6"/>
+      <c r="F20" s="37" t="s">
+        <v>245</v>
+      </c>
       <c r="G20" s="14">
         <v>81</v>
       </c>
@@ -15877,7 +16059,9 @@
       <c r="E21" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="6"/>
+      <c r="F21" s="37" t="s">
+        <v>246</v>
+      </c>
       <c r="G21" s="14">
         <v>86.9</v>
       </c>
@@ -16614,7 +16798,7 @@
       <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="35" t="s">
+      <c r="B22" s="26" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="8">
@@ -16626,7 +16810,9 @@
       <c r="E22" s="7" t="s">
         <v>83</v>
       </c>
-      <c r="F22" s="6"/>
+      <c r="F22" s="37" t="s">
+        <v>247</v>
+      </c>
       <c r="G22" s="14">
         <v>85.75</v>
       </c>
@@ -17373,7 +17559,9 @@
       <c r="E23" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F23" s="6"/>
+      <c r="F23" s="37" t="s">
+        <v>248</v>
+      </c>
       <c r="G23" s="14">
         <v>74.75</v>
       </c>
@@ -18122,7 +18310,9 @@
       <c r="E24" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="6"/>
+      <c r="F24" s="37" t="s">
+        <v>249</v>
+      </c>
       <c r="G24" s="14">
         <v>84.75</v>
       </c>
@@ -18871,7 +19061,9 @@
       <c r="E25" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="37" t="s">
+        <v>250</v>
+      </c>
       <c r="G25" s="14">
         <v>89.7</v>
       </c>
@@ -19620,7 +19812,9 @@
       <c r="E26" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F26" s="6"/>
+      <c r="F26" s="37" t="s">
+        <v>251</v>
+      </c>
       <c r="G26" s="14">
         <v>80</v>
       </c>
@@ -20349,7 +20543,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ26" s="34" t="s">
+      <c r="IJ26" s="25" t="s">
         <v>212</v>
       </c>
     </row>
@@ -20369,7 +20563,9 @@
       <c r="E27" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="F27" s="6"/>
+      <c r="F27" s="37" t="s">
+        <v>252</v>
+      </c>
       <c r="G27" s="14">
         <v>81</v>
       </c>
@@ -21098,7 +21294,7 @@
         <f t="shared" si="16"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="IJ27" s="34" t="s">
+      <c r="IJ27" s="25" t="s">
         <v>213</v>
       </c>
     </row>
@@ -21118,7 +21314,9 @@
       <c r="E28" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="37" t="s">
+        <v>253</v>
+      </c>
       <c r="G28" s="14">
         <v>80</v>
       </c>
@@ -21847,7 +22045,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ28" s="34" t="s">
+      <c r="IJ28" s="25" t="s">
         <v>214</v>
       </c>
     </row>
@@ -21867,7 +22065,9 @@
       <c r="E29" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F29" s="6"/>
+      <c r="F29" s="37" t="s">
+        <v>254</v>
+      </c>
       <c r="G29" s="14">
         <v>82.6</v>
       </c>
@@ -22616,7 +22816,9 @@
       <c r="E30" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="F30" s="6"/>
+      <c r="F30" s="37" t="s">
+        <v>255</v>
+      </c>
       <c r="G30" s="14">
         <v>80</v>
       </c>
@@ -23353,7 +23555,7 @@
       <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="35" t="s">
+      <c r="B31" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="8">
@@ -23365,7 +23567,9 @@
       <c r="E31" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F31" s="6"/>
+      <c r="F31" s="37" t="s">
+        <v>256</v>
+      </c>
       <c r="G31" s="14">
         <v>79</v>
       </c>
@@ -24112,7 +24316,9 @@
       <c r="E32" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="F32" s="6"/>
+      <c r="F32" s="37" t="s">
+        <v>257</v>
+      </c>
       <c r="G32" s="14">
         <v>79.3</v>
       </c>
@@ -24861,7 +25067,9 @@
       <c r="E33" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F33" s="6"/>
+      <c r="F33" s="37" t="s">
+        <v>258</v>
+      </c>
       <c r="G33" s="14">
         <v>84.55</v>
       </c>
@@ -25610,7 +25818,9 @@
       <c r="E34" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="F34" s="6"/>
+      <c r="F34" s="37" t="s">
+        <v>259</v>
+      </c>
       <c r="G34" s="14">
         <v>72.600000000000009</v>
       </c>
@@ -26359,7 +26569,9 @@
       <c r="E35" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F35" s="6"/>
+      <c r="F35" s="37" t="s">
+        <v>260</v>
+      </c>
       <c r="G35" s="14">
         <v>91.35</v>
       </c>
@@ -27108,7 +27320,9 @@
       <c r="E36" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="F36" s="6"/>
+      <c r="F36" s="37" t="s">
+        <v>261</v>
+      </c>
       <c r="G36" s="14">
         <v>82.55</v>
       </c>
@@ -27837,7 +28051,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ36" s="34" t="s">
+      <c r="IJ36" s="25" t="s">
         <v>221</v>
       </c>
     </row>
@@ -27857,7 +28071,9 @@
       <c r="E37" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="6"/>
+      <c r="F37" s="37" t="s">
+        <v>262</v>
+      </c>
       <c r="G37" s="14">
         <v>80.95</v>
       </c>
@@ -28606,7 +28822,9 @@
       <c r="E38" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="6"/>
+      <c r="F38" s="37" t="s">
+        <v>263</v>
+      </c>
       <c r="G38" s="14">
         <v>84.4</v>
       </c>
@@ -29355,7 +29573,9 @@
       <c r="E39" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F39" s="6"/>
+      <c r="F39" s="37" t="s">
+        <v>264</v>
+      </c>
       <c r="G39" s="14">
         <v>87.700000000000017</v>
       </c>
@@ -30104,7 +30324,9 @@
       <c r="E40" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="F40" s="6"/>
+      <c r="F40" s="37" t="s">
+        <v>265</v>
+      </c>
       <c r="G40" s="14">
         <v>86.75</v>
       </c>
@@ -30853,7 +31075,9 @@
       <c r="E41" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="6"/>
+      <c r="F41" s="37" t="s">
+        <v>266</v>
+      </c>
       <c r="G41" s="14">
         <v>85.600000000000009</v>
       </c>
@@ -31602,7 +31826,9 @@
       <c r="E42" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="F42" s="6"/>
+      <c r="F42" s="37" t="s">
+        <v>267</v>
+      </c>
       <c r="G42" s="14">
         <v>86.300000000000011</v>
       </c>
@@ -32339,7 +32565,7 @@
       <c r="A43" s="11">
         <v>41</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="27" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="8">
@@ -32351,7 +32577,9 @@
       <c r="E43" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="F43" s="6"/>
+      <c r="F43" s="37" t="s">
+        <v>268</v>
+      </c>
       <c r="G43" s="14">
         <v>75.149999999999991</v>
       </c>
@@ -33090,61 +33318,6 @@
     </row>
   </sheetData>
   <mergeCells count="68">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="BJ1:BN1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="BE1:BI1"/>
-    <mergeCell ref="DR1:DV1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BT1:BX1"/>
-    <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="CI1:CM1"/>
-    <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="FZ1:GD1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EB1:EF1"/>
-    <mergeCell ref="EG1:EK1"/>
-    <mergeCell ref="EL1:EP1"/>
-    <mergeCell ref="EQ1:EU1"/>
-    <mergeCell ref="EV1:EZ1"/>
-    <mergeCell ref="FA1:FE1"/>
-    <mergeCell ref="FF1:FJ1"/>
-    <mergeCell ref="FK1:FO1"/>
-    <mergeCell ref="FP1:FT1"/>
-    <mergeCell ref="FU1:FY1"/>
-    <mergeCell ref="HI1:HM1"/>
-    <mergeCell ref="HN1:HR1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="GJ1:GN1"/>
-    <mergeCell ref="GO1:GS1"/>
-    <mergeCell ref="GT1:GX1"/>
-    <mergeCell ref="GY1:HC1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="HS1:HS2"/>
-    <mergeCell ref="HU1:HU2"/>
-    <mergeCell ref="HW1:HW2"/>
-    <mergeCell ref="HY1:HY2"/>
-    <mergeCell ref="IA1:IA2"/>
     <mergeCell ref="II1:II2"/>
     <mergeCell ref="IJ1:IJ2"/>
     <mergeCell ref="HT1:HT2"/>
@@ -33158,7 +33331,63 @@
     <mergeCell ref="IF1:IF2"/>
     <mergeCell ref="IE1:IE2"/>
     <mergeCell ref="IH1:IH2"/>
+    <mergeCell ref="HS1:HS2"/>
+    <mergeCell ref="HU1:HU2"/>
+    <mergeCell ref="HW1:HW2"/>
+    <mergeCell ref="HY1:HY2"/>
+    <mergeCell ref="IA1:IA2"/>
+    <mergeCell ref="HI1:HM1"/>
+    <mergeCell ref="HN1:HR1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="GJ1:GN1"/>
+    <mergeCell ref="GO1:GS1"/>
+    <mergeCell ref="GT1:GX1"/>
+    <mergeCell ref="GY1:HC1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FZ1:GD1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EB1:EF1"/>
+    <mergeCell ref="EG1:EK1"/>
+    <mergeCell ref="EL1:EP1"/>
+    <mergeCell ref="EQ1:EU1"/>
+    <mergeCell ref="EV1:EZ1"/>
+    <mergeCell ref="FA1:FE1"/>
+    <mergeCell ref="FF1:FJ1"/>
+    <mergeCell ref="FK1:FO1"/>
+    <mergeCell ref="FP1:FT1"/>
+    <mergeCell ref="FU1:FY1"/>
+    <mergeCell ref="DR1:DV1"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="BT1:BX1"/>
+    <mergeCell ref="BY1:CC1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="CI1:CM1"/>
+    <mergeCell ref="CN1:CR1"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DH1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BE1:BI1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
revisi template d3 dan s1 reguler besar2an
</commit_message>
<xml_diff>
--- a/D3 Keperawatan/Transkip Nilai D3 Kep.xlsx
+++ b/D3 Keperawatan/Transkip Nilai D3 Kep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\D3 Keperawatan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB054F8-0D0E-4B60-8606-011A1BEB6810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9F06DD-347F-4C62-8E13-E66F29712585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22668FF5-9BBF-4EB6-990E-3DE3502F0C5B}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2301" uniqueCount="271">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2340" uniqueCount="310">
   <si>
     <t>NO</t>
   </si>
@@ -615,9 +615,6 @@
     <t>Implementasi Terapi Ankle Pumping Exercise Dengan Elevasi Kaki 30° Untuk Menurunkan Edema Pada Pasien Gagal Ginjal Kronik (Ggk) Di Rsal Dr. Midiyato Suratani Kota Tanjungpinang</t>
   </si>
   <si>
-    <t>Laporan Karya Tulis Ilmiah Implementasi Pengunaan Spalk Bermotif Pada An.S Untuk Menurunkan Tingkat Kecemasan Saat Pemasangan Infus Di Rungan Subi Rsal Dr.Midiyato Suratani</t>
-  </si>
-  <si>
     <t>Implementasi Chest Fisioterapi Clapping Pada An.N Dengan Bersihan Jalan Nafas Tidak Efektif di Ruang Subi Kecil Rumkital Dr. Midiyato Suratani Kota Tanjungpinang</t>
   </si>
   <si>
@@ -848,6 +845,126 @@
   <si>
     <t>15 Mei 2005</t>
   </si>
+  <si>
+    <t>Judul Inggris</t>
+  </si>
+  <si>
+    <t>Implementation of Complementary Foot Massage Therapy Using Olive Oil in the Family of Mr. K with Hypertension: Risk of Ineffective Peripheral Perfusion in the Working Area of Tanjungpinang Health Center</t>
+  </si>
+  <si>
+    <t>Implementation of Chewing Gum Therapy for Mrs. D to Reduce Thirst in Chronic Kidney Disease Patients Undergoing Hemodialysis at Dr. Midiyato Suratani Naval Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Ankle Pumping Exercise with 30° Leg Elevation as an Intervention to Decrease Edema in Chronic Kidney Disease (CKD) Patients: Implementation at Dr. Midiyato Suratani Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Laporan Karya Tulis Ilmiah Implementasi Pengunaan Spalk Bermotif Pada An.S Untuk Menurunkan Tingkat Kecemasan Saat Pemasangan Infus Di Ruangan Subi Rsal Dr.Midiyato Suratani</t>
+  </si>
+  <si>
+    <t>Scientific Writing Report: Implementation of Patterned Splint Application for Reducing Anxiety During IV Insertion in Pediatric Patient S at the Subi Ward, Dr. Midiyato Suratani Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Chest Physiotherapy Clapping Technique for Child N with Ineffective Airway Clearance in the Subi Mini Room of Dr. Midiyato Suratani Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of FAST Therapy and 30° Head-Up Positioning in Stroke Patients with Ineffective Cerebral Perfusion in the Intensive Care Unit (ICU) of BLUD Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Progressive Muscle Relaxation Therapy to Reduce Headache in Elderly Patients with Hypertension at the Social Services Office of Tanjungpinang City</t>
+  </si>
+  <si>
+    <t>Implementation of Rhythmic Breathing Distraction for Ms. A After Appendectomy with Acute Pain in the Bougenville Room, Tanjungpinang City General Hospital (RSUD)</t>
+  </si>
+  <si>
+    <t>Implementation of Progressive Muscle Relaxation in Mr. F with Risk of Violent Behavior at Engku Haji Daud Mental Hospital, Tanjung Uban</t>
+  </si>
+  <si>
+    <t>Implementation of Progressive Muscle Relaxation for Ms. R After Breast Cancer Surgery with Sleep Pattern Disturbance in the Bougenville Room, Tanjungpinang City Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Foot Massage Therapy for Chronic Pain Reduction in Mrs. M with Rheumatoid Arthritis at Embung Fatimah Nursing Home, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Early Mobilization and Slow Deep Breathing Techniques for Pain Reduction in Appendectomy Patients in the Bougenvile Room, Tanjungpinang City Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Mozart Classical Music Therapy in Controlling Auditory Hallucinations in Mr. A with Schizophrenia at Engku Haji Daud Hospital, Tanjung Uban</t>
+  </si>
+  <si>
+    <t>Implementation of Warm Foot Bath and Slow Deep Breathing Therapy for Hypertensive Patients at Risk of Ineffective Peripheral Perfusion in the Dahlia Room, Tanjungpinang City Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Spiky Rubber Ball Grip Therapy for Elderly Stroke Patients with Left Hemiparesis and Physical Mobility Impairment at Rumah Bahagia Binta</t>
+  </si>
+  <si>
+    <t>Implementation of Foot Massage Therapy in Mrs. N After Cesarean Section with Acute Pain in the Cempaka Room, BLUD Hospital Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of 0.9% Normal Saline Compress for Reducing Phlebitis Pain in Pediatric Patient R in the Flamboyan Room, Tanjungpinang City Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Eucalyptus Oil Vapor Inhalation Therapy for Child U with Bronchopneumonia and Ineffective Airway Clearance in the Flamboyan Room, BLUD Hospital Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of the Kangaroo Method to Increase Body Temperature in Hypothermic Low-Birth-Weight Infant of Mrs. P in the NICU of BLUD Tanjungpinang City Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Balloon Blowing Technique in Mr. L with Ineffective Airway Clearance in the Dahlia Ward of BLUD Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Classical Music Therapy for Mr. A Post–Inguinal Hernia Surgery with Acute Pain in the Bougenville Ward of BLUD Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Woolwich Massage and Quranic Murottal Relaxation for Postpartum Mothers Experiencing Ineffective Breastfeeding in the Cempaka Room, Tanjungpinang City Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Classical Music Auditory Distraction Therapy for Mr. A with Anxiety in the Damar Room, Dr. Midiyato Suratani Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Puzzle-Based Play Therapy for Anxiety Management in Pediatric Patient S in the Subi Room, Dr. Midiyato Suratani Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Lego Play Therapy in Child Y to Reduce Anxiety Levels in Toddlers During Hospitalization in the Subi Kecil Ward of Dr. Midiyato Suratani Naval Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Menstrual Pads in Perineal Wound Care for Mrs. Y Post Spontaneous Delivery with Infection Risk in Cempaka Ward, RS-BLUD Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Pursed Lips Breathing Exercise (Balloon Blowing) to Improve Oxygen Needs in Child A with Bronchopneumonia in the Flamboyan Ward of RSUD Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Mozart Classical Music Therapy for Mr. R with Risk of Violent Behavior at Engku Haji Daud Psychiatric Hospital (RSJKO), Tanjung Uban, Riau Islands Province</t>
+  </si>
+  <si>
+    <t>Implementation of Thermotherapy for Acute Pain in Mr. S with Acute Coronary Syndrome (ACS) in the Damar Ward of Dr. Midiyato Suratani Naval Hospital, Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Audiovisual Distraction Techniques Using Cartoon Films During Injection Procedures to Reduce Anxiety in Child R in the Subi Kecil Room of Dr. Midiyato Naval Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Diabetic Foot Exercise in Clients With Diabetic Ulcers and Ineffective Peripheral Tissue Perfusion in the Bougenville Ward of Tanjungpinang General Hospital</t>
+  </si>
+  <si>
+    <t>mplementation of Nursing Care Using Drawing Therapy for Schizophrenia Patients With Auditory Hallucinations in the Flamboyan A Ward of Engku Haji Daud Psychiatric Hospital, Riau Islands Province</t>
+  </si>
+  <si>
+    <t>Implementation of Positive Affirmation Therapy to Improve Self-Esteem in Clients With Chronic Low Self-Esteem in the Flamboyan Ward of Engku Haji Daud Psychiatric Hospital, Tanjung Uban</t>
+  </si>
+  <si>
+    <t>Implementation of Hand-Holding Therapy for Hypertension Patients With Acute Pain in the Dahlia Ward of RS-BLUD Tanjungpinang</t>
+  </si>
+  <si>
+    <t>Implementation of Progressive Muscle Relaxation and Slow Stroke Back Massage to Reduce Blood Pressure in Elderly Patients With Hypertension at the Social Services Office of Tanjungpinang City</t>
+  </si>
+  <si>
+    <t>Implementation of Token Economy Behavioral Therapy for Schizophrenia Patients With Self-Care Deficit in the Flamboyan A Ward of RSJKO Engku Haji Daud, Riau Islands Province</t>
+  </si>
+  <si>
+    <t>Implementation of Diabetes Mellitus Foot Care Education Through Video Media for the Prevention of Diabetic Ulcers in Patients With Knowledge Deficit at Tanjungpinang City General Hospital</t>
+  </si>
+  <si>
+    <t>Implementation of Balance Exercises for the Elderly at Rumah Bahagia Embung Fatimah, Tanjungpinang City</t>
+  </si>
 </sst>
 </file>
 
@@ -1025,7 +1142,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1085,9 +1202,6 @@
     <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1097,20 +1211,11 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1118,12 +1223,25 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good 2" xfId="4" xr:uid="{9E58217C-29C0-4F6B-BCCA-FBD9D11D267D}"/>
@@ -1442,13 +1560,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2967CDF3-E1DE-4ED6-83C3-5F7B380BED6A}">
-  <dimension ref="A1:IJ44"/>
+  <dimension ref="A1:IK44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="HS3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="2" topLeftCell="IF30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37:XFD37"/>
+      <selection pane="bottomRight" activeCell="IK42" sqref="IK42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1463,146 +1581,147 @@
     <col min="242" max="242" width="27.5703125" customWidth="1"/>
     <col min="243" max="243" width="24.28515625" style="1" customWidth="1"/>
     <col min="244" max="244" width="18.85546875" customWidth="1"/>
+    <col min="245" max="245" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:244" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+    <row r="1" spans="1:245" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="35" t="s">
+      <c r="G1" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35"/>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35" t="s">
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="35"/>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35"/>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35" t="s">
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
+      <c r="Q1" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="R1" s="35"/>
-      <c r="S1" s="35"/>
-      <c r="T1" s="35"/>
-      <c r="U1" s="35"/>
-      <c r="V1" s="35" t="s">
+      <c r="R1" s="31"/>
+      <c r="S1" s="31"/>
+      <c r="T1" s="31"/>
+      <c r="U1" s="31"/>
+      <c r="V1" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="W1" s="35"/>
-      <c r="X1" s="35"/>
-      <c r="Y1" s="35"/>
-      <c r="Z1" s="35"/>
-      <c r="AA1" s="35" t="s">
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="35"/>
-      <c r="AC1" s="35"/>
-      <c r="AD1" s="35"/>
-      <c r="AE1" s="35"/>
-      <c r="AF1" s="35" t="s">
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="AG1" s="35"/>
-      <c r="AH1" s="35"/>
-      <c r="AI1" s="35"/>
-      <c r="AJ1" s="35"/>
-      <c r="AK1" s="35" t="s">
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="AL1" s="35"/>
-      <c r="AM1" s="35"/>
-      <c r="AN1" s="35"/>
-      <c r="AO1" s="35"/>
-      <c r="AP1" s="35" t="s">
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31" t="s">
         <v>126</v>
       </c>
-      <c r="AQ1" s="35"/>
-      <c r="AR1" s="35"/>
-      <c r="AS1" s="35"/>
-      <c r="AT1" s="35"/>
-      <c r="AU1" s="35" t="s">
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31" t="s">
         <v>127</v>
       </c>
-      <c r="AV1" s="35"/>
-      <c r="AW1" s="35"/>
-      <c r="AX1" s="35"/>
-      <c r="AY1" s="35"/>
-      <c r="AZ1" s="34" t="s">
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="BA1" s="34"/>
-      <c r="BB1" s="34"/>
-      <c r="BC1" s="34"/>
-      <c r="BD1" s="34"/>
-      <c r="BE1" s="34" t="s">
+      <c r="BA1" s="30"/>
+      <c r="BB1" s="30"/>
+      <c r="BC1" s="30"/>
+      <c r="BD1" s="30"/>
+      <c r="BE1" s="30" t="s">
         <v>129</v>
       </c>
-      <c r="BF1" s="34"/>
-      <c r="BG1" s="34"/>
-      <c r="BH1" s="34"/>
-      <c r="BI1" s="34"/>
-      <c r="BJ1" s="34" t="s">
+      <c r="BF1" s="30"/>
+      <c r="BG1" s="30"/>
+      <c r="BH1" s="30"/>
+      <c r="BI1" s="30"/>
+      <c r="BJ1" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="BK1" s="34"/>
-      <c r="BL1" s="34"/>
-      <c r="BM1" s="34"/>
-      <c r="BN1" s="34"/>
-      <c r="BO1" s="34" t="s">
+      <c r="BK1" s="30"/>
+      <c r="BL1" s="30"/>
+      <c r="BM1" s="30"/>
+      <c r="BN1" s="30"/>
+      <c r="BO1" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="BP1" s="34"/>
-      <c r="BQ1" s="34"/>
-      <c r="BR1" s="34"/>
-      <c r="BS1" s="34"/>
-      <c r="BT1" s="34" t="s">
+      <c r="BP1" s="30"/>
+      <c r="BQ1" s="30"/>
+      <c r="BR1" s="30"/>
+      <c r="BS1" s="30"/>
+      <c r="BT1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="BU1" s="34"/>
-      <c r="BV1" s="34"/>
-      <c r="BW1" s="34"/>
-      <c r="BX1" s="34"/>
-      <c r="BY1" s="34" t="s">
+      <c r="BU1" s="30"/>
+      <c r="BV1" s="30"/>
+      <c r="BW1" s="30"/>
+      <c r="BX1" s="30"/>
+      <c r="BY1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="BZ1" s="34"/>
-      <c r="CA1" s="34"/>
-      <c r="CB1" s="34"/>
-      <c r="CC1" s="34"/>
-      <c r="CD1" s="34" t="s">
+      <c r="BZ1" s="30"/>
+      <c r="CA1" s="30"/>
+      <c r="CB1" s="30"/>
+      <c r="CC1" s="30"/>
+      <c r="CD1" s="30" t="s">
         <v>134</v>
       </c>
-      <c r="CE1" s="34"/>
-      <c r="CF1" s="34"/>
-      <c r="CG1" s="34"/>
-      <c r="CH1" s="34"/>
-      <c r="CI1" s="34" t="s">
+      <c r="CE1" s="30"/>
+      <c r="CF1" s="30"/>
+      <c r="CG1" s="30"/>
+      <c r="CH1" s="30"/>
+      <c r="CI1" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="CJ1" s="34"/>
-      <c r="CK1" s="34"/>
-      <c r="CL1" s="34"/>
-      <c r="CM1" s="34"/>
+      <c r="CJ1" s="30"/>
+      <c r="CK1" s="30"/>
+      <c r="CL1" s="30"/>
+      <c r="CM1" s="30"/>
       <c r="CN1" s="32" t="s">
         <v>138</v>
       </c>
@@ -1659,201 +1778,204 @@
       <c r="DY1" s="32"/>
       <c r="DZ1" s="32"/>
       <c r="EA1" s="32"/>
-      <c r="EB1" s="33" t="s">
+      <c r="EB1" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="EC1" s="33"/>
-      <c r="ED1" s="33"/>
-      <c r="EE1" s="33"/>
-      <c r="EF1" s="33"/>
-      <c r="EG1" s="33" t="s">
+      <c r="EC1" s="34"/>
+      <c r="ED1" s="34"/>
+      <c r="EE1" s="34"/>
+      <c r="EF1" s="34"/>
+      <c r="EG1" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="EH1" s="33"/>
-      <c r="EI1" s="33"/>
-      <c r="EJ1" s="33"/>
-      <c r="EK1" s="33"/>
-      <c r="EL1" s="33" t="s">
+      <c r="EH1" s="34"/>
+      <c r="EI1" s="34"/>
+      <c r="EJ1" s="34"/>
+      <c r="EK1" s="34"/>
+      <c r="EL1" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="EM1" s="33"/>
-      <c r="EN1" s="33"/>
-      <c r="EO1" s="33"/>
-      <c r="EP1" s="33"/>
-      <c r="EQ1" s="33" t="s">
+      <c r="EM1" s="34"/>
+      <c r="EN1" s="34"/>
+      <c r="EO1" s="34"/>
+      <c r="EP1" s="34"/>
+      <c r="EQ1" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="ER1" s="33"/>
-      <c r="ES1" s="33"/>
-      <c r="ET1" s="33"/>
-      <c r="EU1" s="33"/>
-      <c r="EV1" s="33" t="s">
+      <c r="ER1" s="34"/>
+      <c r="ES1" s="34"/>
+      <c r="ET1" s="34"/>
+      <c r="EU1" s="34"/>
+      <c r="EV1" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="EW1" s="33"/>
-      <c r="EX1" s="33"/>
-      <c r="EY1" s="33"/>
-      <c r="EZ1" s="33"/>
-      <c r="FA1" s="33" t="s">
+      <c r="EW1" s="34"/>
+      <c r="EX1" s="34"/>
+      <c r="EY1" s="34"/>
+      <c r="EZ1" s="34"/>
+      <c r="FA1" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="FB1" s="33"/>
-      <c r="FC1" s="33"/>
-      <c r="FD1" s="33"/>
-      <c r="FE1" s="33"/>
-      <c r="FF1" s="33" t="s">
+      <c r="FB1" s="34"/>
+      <c r="FC1" s="34"/>
+      <c r="FD1" s="34"/>
+      <c r="FE1" s="34"/>
+      <c r="FF1" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="FG1" s="33"/>
-      <c r="FH1" s="33"/>
-      <c r="FI1" s="33"/>
-      <c r="FJ1" s="33"/>
-      <c r="FK1" s="33" t="s">
+      <c r="FG1" s="34"/>
+      <c r="FH1" s="34"/>
+      <c r="FI1" s="34"/>
+      <c r="FJ1" s="34"/>
+      <c r="FK1" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="FL1" s="33"/>
-      <c r="FM1" s="33"/>
-      <c r="FN1" s="33"/>
-      <c r="FO1" s="33"/>
-      <c r="FP1" s="31" t="s">
+      <c r="FL1" s="34"/>
+      <c r="FM1" s="34"/>
+      <c r="FN1" s="34"/>
+      <c r="FO1" s="34"/>
+      <c r="FP1" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="FQ1" s="31"/>
-      <c r="FR1" s="31"/>
-      <c r="FS1" s="31"/>
-      <c r="FT1" s="31"/>
-      <c r="FU1" s="31" t="s">
+      <c r="FQ1" s="33"/>
+      <c r="FR1" s="33"/>
+      <c r="FS1" s="33"/>
+      <c r="FT1" s="33"/>
+      <c r="FU1" s="33" t="s">
         <v>156</v>
       </c>
-      <c r="FV1" s="31"/>
-      <c r="FW1" s="31"/>
-      <c r="FX1" s="31"/>
-      <c r="FY1" s="31"/>
-      <c r="FZ1" s="31" t="s">
+      <c r="FV1" s="33"/>
+      <c r="FW1" s="33"/>
+      <c r="FX1" s="33"/>
+      <c r="FY1" s="33"/>
+      <c r="FZ1" s="33" t="s">
         <v>157</v>
       </c>
-      <c r="GA1" s="31"/>
-      <c r="GB1" s="31"/>
-      <c r="GC1" s="31"/>
-      <c r="GD1" s="31"/>
-      <c r="GE1" s="31" t="s">
+      <c r="GA1" s="33"/>
+      <c r="GB1" s="33"/>
+      <c r="GC1" s="33"/>
+      <c r="GD1" s="33"/>
+      <c r="GE1" s="33" t="s">
         <v>158</v>
       </c>
-      <c r="GF1" s="31"/>
-      <c r="GG1" s="31"/>
-      <c r="GH1" s="31"/>
-      <c r="GI1" s="31"/>
-      <c r="GJ1" s="31" t="s">
+      <c r="GF1" s="33"/>
+      <c r="GG1" s="33"/>
+      <c r="GH1" s="33"/>
+      <c r="GI1" s="33"/>
+      <c r="GJ1" s="33" t="s">
         <v>159</v>
       </c>
-      <c r="GK1" s="31"/>
-      <c r="GL1" s="31"/>
-      <c r="GM1" s="31"/>
-      <c r="GN1" s="31"/>
-      <c r="GO1" s="31" t="s">
+      <c r="GK1" s="33"/>
+      <c r="GL1" s="33"/>
+      <c r="GM1" s="33"/>
+      <c r="GN1" s="33"/>
+      <c r="GO1" s="33" t="s">
         <v>160</v>
       </c>
-      <c r="GP1" s="31"/>
-      <c r="GQ1" s="31"/>
-      <c r="GR1" s="31"/>
-      <c r="GS1" s="31"/>
-      <c r="GT1" s="31" t="s">
+      <c r="GP1" s="33"/>
+      <c r="GQ1" s="33"/>
+      <c r="GR1" s="33"/>
+      <c r="GS1" s="33"/>
+      <c r="GT1" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="GU1" s="31"/>
-      <c r="GV1" s="31"/>
-      <c r="GW1" s="31"/>
-      <c r="GX1" s="31"/>
-      <c r="GY1" s="31" t="s">
+      <c r="GU1" s="33"/>
+      <c r="GV1" s="33"/>
+      <c r="GW1" s="33"/>
+      <c r="GX1" s="33"/>
+      <c r="GY1" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="GZ1" s="31"/>
-      <c r="HA1" s="31"/>
-      <c r="HB1" s="31"/>
-      <c r="HC1" s="31"/>
-      <c r="HD1" s="31" t="s">
+      <c r="GZ1" s="33"/>
+      <c r="HA1" s="33"/>
+      <c r="HB1" s="33"/>
+      <c r="HC1" s="33"/>
+      <c r="HD1" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="HE1" s="31"/>
-      <c r="HF1" s="31"/>
-      <c r="HG1" s="31"/>
-      <c r="HH1" s="31"/>
-      <c r="HI1" s="30" t="s">
+      <c r="HE1" s="33"/>
+      <c r="HF1" s="33"/>
+      <c r="HG1" s="33"/>
+      <c r="HH1" s="33"/>
+      <c r="HI1" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="HJ1" s="30"/>
-      <c r="HK1" s="30"/>
-      <c r="HL1" s="30"/>
-      <c r="HM1" s="30"/>
-      <c r="HN1" s="30" t="s">
+      <c r="HJ1" s="35"/>
+      <c r="HK1" s="35"/>
+      <c r="HL1" s="35"/>
+      <c r="HM1" s="35"/>
+      <c r="HN1" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="HO1" s="30"/>
-      <c r="HP1" s="30"/>
-      <c r="HQ1" s="30"/>
-      <c r="HR1" s="30"/>
-      <c r="HS1" s="29" t="s">
+      <c r="HO1" s="35"/>
+      <c r="HP1" s="35"/>
+      <c r="HQ1" s="35"/>
+      <c r="HR1" s="35"/>
+      <c r="HS1" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="HT1" s="29" t="s">
+      <c r="HT1" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="HU1" s="29" t="s">
+      <c r="HU1" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="HV1" s="29" t="s">
+      <c r="HV1" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="HW1" s="29" t="s">
+      <c r="HW1" s="36" t="s">
         <v>185</v>
       </c>
-      <c r="HX1" s="29" t="s">
+      <c r="HX1" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="HY1" s="29" t="s">
+      <c r="HY1" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="HZ1" s="29" t="s">
+      <c r="HZ1" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="IA1" s="29" t="s">
+      <c r="IA1" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="IB1" s="29" t="s">
+      <c r="IB1" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="IC1" s="29" t="s">
+      <c r="IC1" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="ID1" s="29" t="s">
+      <c r="ID1" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="IE1" s="29" t="s">
+      <c r="IE1" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="IF1" s="29" t="s">
+      <c r="IF1" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="IG1" s="29" t="s">
+      <c r="IG1" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="IH1" s="29" t="s">
+      <c r="IH1" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="II1" s="29" t="s">
+      <c r="II1" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="IJ1" s="29" t="s">
+      <c r="IJ1" s="36" t="s">
         <v>176</v>
       </c>
+      <c r="IK1" s="36" t="s">
+        <v>270</v>
+      </c>
     </row>
-    <row r="2" spans="1:244" x14ac:dyDescent="0.25">
-      <c r="A2" s="36"/>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="36"/>
+    <row r="2" spans="1:245" x14ac:dyDescent="0.25">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="28"/>
       <c r="G2" s="10" t="s">
         <v>44</v>
       </c>
@@ -2514,26 +2636,27 @@
       <c r="HR2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="HS2" s="29"/>
-      <c r="HT2" s="29"/>
-      <c r="HU2" s="29"/>
-      <c r="HV2" s="29"/>
-      <c r="HW2" s="29"/>
-      <c r="HX2" s="29"/>
-      <c r="HY2" s="29"/>
-      <c r="HZ2" s="29"/>
-      <c r="IA2" s="29"/>
-      <c r="IB2" s="29"/>
-      <c r="IC2" s="29"/>
-      <c r="ID2" s="29"/>
-      <c r="IE2" s="29"/>
-      <c r="IF2" s="29"/>
-      <c r="IG2" s="29"/>
-      <c r="IH2" s="29"/>
-      <c r="II2" s="29"/>
-      <c r="IJ2" s="29"/>
+      <c r="HS2" s="36"/>
+      <c r="HT2" s="36"/>
+      <c r="HU2" s="36"/>
+      <c r="HV2" s="36"/>
+      <c r="HW2" s="36"/>
+      <c r="HX2" s="36"/>
+      <c r="HY2" s="36"/>
+      <c r="HZ2" s="36"/>
+      <c r="IA2" s="36"/>
+      <c r="IB2" s="36"/>
+      <c r="IC2" s="36"/>
+      <c r="ID2" s="36"/>
+      <c r="IE2" s="36"/>
+      <c r="IF2" s="36"/>
+      <c r="IG2" s="36"/>
+      <c r="IH2" s="36"/>
+      <c r="II2" s="36"/>
+      <c r="IJ2" s="36"/>
+      <c r="IK2" s="36"/>
     </row>
-    <row r="3" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
         <v>1</v>
       </c>
@@ -2549,8 +2672,8 @@
       <c r="E3" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>226</v>
+      <c r="F3" s="27" t="s">
+        <v>225</v>
       </c>
       <c r="G3" s="14">
         <v>87.6</v>
@@ -3283,8 +3406,11 @@
       <c r="IJ3" s="3" t="s">
         <v>190</v>
       </c>
+      <c r="IK3" s="38" t="s">
+        <v>271</v>
+      </c>
     </row>
-    <row r="4" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A4" s="11">
         <v>2</v>
       </c>
@@ -3300,8 +3426,8 @@
       <c r="E4" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>227</v>
+      <c r="F4" s="27" t="s">
+        <v>226</v>
       </c>
       <c r="G4" s="14">
         <v>84.6</v>
@@ -4034,8 +4160,11 @@
       <c r="IJ4" s="3" t="s">
         <v>191</v>
       </c>
+      <c r="IK4" s="3" t="s">
+        <v>272</v>
+      </c>
     </row>
-    <row r="5" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A5" s="11">
         <v>3</v>
       </c>
@@ -4051,8 +4180,8 @@
       <c r="E5" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="28" t="s">
-        <v>228</v>
+      <c r="F5" s="27" t="s">
+        <v>227</v>
       </c>
       <c r="G5" s="14">
         <v>85.35</v>
@@ -4783,8 +4912,11 @@
       <c r="IJ5" s="3" t="s">
         <v>192</v>
       </c>
+      <c r="IK5" s="3" t="s">
+        <v>273</v>
+      </c>
     </row>
-    <row r="6" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A6" s="11">
         <v>4</v>
       </c>
@@ -4800,8 +4932,8 @@
       <c r="E6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="F6" s="28" t="s">
-        <v>229</v>
+      <c r="F6" s="27" t="s">
+        <v>228</v>
       </c>
       <c r="G6" s="14">
         <v>86.15</v>
@@ -5532,10 +5664,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ6" s="3" t="s">
-        <v>193</v>
+        <v>274</v>
+      </c>
+      <c r="IK6" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
-    <row r="7" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A7" s="11">
         <v>5</v>
       </c>
@@ -5551,8 +5686,8 @@
       <c r="E7" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="28" t="s">
-        <v>230</v>
+      <c r="F7" s="27" t="s">
+        <v>229</v>
       </c>
       <c r="G7" s="14">
         <v>86.95</v>
@@ -6283,10 +6418,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ7" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
+      </c>
+      <c r="IK7" s="3" t="s">
+        <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A8" s="11">
         <v>6</v>
       </c>
@@ -6302,8 +6440,8 @@
       <c r="E8" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="28" t="s">
-        <v>231</v>
+      <c r="F8" s="27" t="s">
+        <v>230</v>
       </c>
       <c r="G8" s="14">
         <v>82.3</v>
@@ -7034,10 +7172,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ8" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
+      </c>
+      <c r="IK8" s="3" t="s">
+        <v>277</v>
       </c>
     </row>
-    <row r="9" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A9" s="11">
         <v>7</v>
       </c>
@@ -7053,8 +7194,8 @@
       <c r="E9" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F9" s="28" t="s">
-        <v>232</v>
+      <c r="F9" s="27" t="s">
+        <v>231</v>
       </c>
       <c r="G9" s="14">
         <v>84.1</v>
@@ -7785,10 +7926,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ9" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
+      </c>
+      <c r="IK9" s="3" t="s">
+        <v>278</v>
       </c>
     </row>
-    <row r="10" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A10" s="11">
         <v>8</v>
       </c>
@@ -7804,8 +7948,8 @@
       <c r="E10" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="28" t="s">
-        <v>233</v>
+      <c r="F10" s="27" t="s">
+        <v>232</v>
       </c>
       <c r="G10" s="14">
         <v>82.6</v>
@@ -8536,10 +8680,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ10" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
+      </c>
+      <c r="IK10" s="3" t="s">
+        <v>279</v>
       </c>
     </row>
-    <row r="11" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A11" s="11">
         <v>9</v>
       </c>
@@ -8555,8 +8702,8 @@
       <c r="E11" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="28" t="s">
-        <v>234</v>
+      <c r="F11" s="27" t="s">
+        <v>233</v>
       </c>
       <c r="G11" s="14">
         <v>79</v>
@@ -9287,10 +9434,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ11" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
+      </c>
+      <c r="IK11" s="3" t="s">
+        <v>280</v>
       </c>
     </row>
-    <row r="12" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A12" s="11">
         <v>10</v>
       </c>
@@ -9306,8 +9456,8 @@
       <c r="E12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="28" t="s">
-        <v>235</v>
+      <c r="F12" s="27" t="s">
+        <v>234</v>
       </c>
       <c r="G12" s="14">
         <v>86.450000000000017</v>
@@ -10038,10 +10188,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ12" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
+      </c>
+      <c r="IK12" s="3" t="s">
+        <v>281</v>
       </c>
     </row>
-    <row r="13" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A13" s="11">
         <v>11</v>
       </c>
@@ -10055,10 +10208,10 @@
         <v>66</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="F13" s="28" t="s">
-        <v>236</v>
+        <v>269</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>235</v>
       </c>
       <c r="G13" s="14">
         <v>91.35</v>
@@ -10789,10 +10942,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ13" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
+      </c>
+      <c r="IK13" s="3" t="s">
+        <v>282</v>
       </c>
     </row>
-    <row r="14" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A14" s="11">
         <v>12</v>
       </c>
@@ -10808,8 +10964,8 @@
       <c r="E14" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="28" t="s">
-        <v>237</v>
+      <c r="F14" s="27" t="s">
+        <v>236</v>
       </c>
       <c r="G14" s="14">
         <v>88.1</v>
@@ -11540,10 +11696,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ14" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
+      </c>
+      <c r="IK14" s="3" t="s">
+        <v>283</v>
       </c>
     </row>
-    <row r="15" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A15" s="11">
         <v>13</v>
       </c>
@@ -11559,8 +11718,8 @@
       <c r="E15" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F15" s="28" t="s">
-        <v>238</v>
+      <c r="F15" s="27" t="s">
+        <v>237</v>
       </c>
       <c r="G15" s="14">
         <v>85</v>
@@ -12291,10 +12450,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ15" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
+      </c>
+      <c r="IK15" s="3" t="s">
+        <v>284</v>
       </c>
     </row>
-    <row r="16" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A16" s="11">
         <v>14</v>
       </c>
@@ -12310,8 +12472,8 @@
       <c r="E16" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="F16" s="28" t="s">
-        <v>239</v>
+      <c r="F16" s="27" t="s">
+        <v>238</v>
       </c>
       <c r="G16" s="14">
         <v>86.05</v>
@@ -13041,11 +13203,14 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ16" s="25" t="s">
-        <v>202</v>
+      <c r="IJ16" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="IK16" s="3" t="s">
+        <v>285</v>
       </c>
     </row>
-    <row r="17" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>15</v>
       </c>
@@ -13061,8 +13226,8 @@
       <c r="E17" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="28" t="s">
-        <v>240</v>
+      <c r="F17" s="27" t="s">
+        <v>239</v>
       </c>
       <c r="G17" s="14">
         <v>85.6</v>
@@ -13793,10 +13958,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ17" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
+      </c>
+      <c r="IK17" s="3" t="s">
+        <v>286</v>
       </c>
     </row>
-    <row r="18" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A18" s="11">
         <v>16</v>
       </c>
@@ -13812,8 +13980,8 @@
       <c r="E18" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="F18" s="28" t="s">
-        <v>241</v>
+      <c r="F18" s="27" t="s">
+        <v>240</v>
       </c>
       <c r="G18" s="14">
         <v>87.6</v>
@@ -14544,10 +14712,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ18" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
+      </c>
+      <c r="IK18" s="3" t="s">
+        <v>287</v>
       </c>
     </row>
-    <row r="19" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A19" s="11">
         <v>17</v>
       </c>
@@ -14563,8 +14734,8 @@
       <c r="E19" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="28" t="s">
-        <v>242</v>
+      <c r="F19" s="27" t="s">
+        <v>241</v>
       </c>
       <c r="G19" s="14">
         <v>88.85</v>
@@ -15295,10 +15466,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ19" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
+      </c>
+      <c r="IK19" s="3" t="s">
+        <v>288</v>
       </c>
     </row>
-    <row r="20" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A20" s="11">
         <v>18</v>
       </c>
@@ -15314,8 +15488,8 @@
       <c r="E20" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="F20" s="28" t="s">
-        <v>243</v>
+      <c r="F20" s="27" t="s">
+        <v>242</v>
       </c>
       <c r="G20" s="14">
         <v>81</v>
@@ -16046,10 +16220,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ20" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
+      </c>
+      <c r="IK20" s="3" t="s">
+        <v>289</v>
       </c>
     </row>
-    <row r="21" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A21" s="11">
         <v>19</v>
       </c>
@@ -16065,8 +16242,8 @@
       <c r="E21" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="F21" s="28" t="s">
-        <v>244</v>
+      <c r="F21" s="27" t="s">
+        <v>243</v>
       </c>
       <c r="G21" s="14">
         <v>86.9</v>
@@ -16797,14 +16974,17 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ21" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
+      </c>
+      <c r="IK21" s="3" t="s">
+        <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A22" s="11">
         <v>20</v>
       </c>
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C22" s="8">
@@ -16816,8 +16996,8 @@
       <c r="E22" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="28" t="s">
-        <v>245</v>
+      <c r="F22" s="27" t="s">
+        <v>244</v>
       </c>
       <c r="G22" s="14">
         <v>85.75</v>
@@ -17548,8 +17728,9 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ22" s="3"/>
+      <c r="IK22" s="3"/>
     </row>
-    <row r="23" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A23" s="11">
         <v>21</v>
       </c>
@@ -17565,8 +17746,8 @@
       <c r="E23" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="F23" s="28" t="s">
-        <v>246</v>
+      <c r="F23" s="27" t="s">
+        <v>245</v>
       </c>
       <c r="G23" s="14">
         <v>74.75</v>
@@ -18297,10 +18478,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ23" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
+      </c>
+      <c r="IK23" s="3" t="s">
+        <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A24" s="11">
         <v>22</v>
       </c>
@@ -18316,8 +18500,8 @@
       <c r="E24" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="28" t="s">
-        <v>247</v>
+      <c r="F24" s="27" t="s">
+        <v>246</v>
       </c>
       <c r="G24" s="14">
         <v>84.75</v>
@@ -19048,10 +19232,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ24" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
+      </c>
+      <c r="IK24" s="3" t="s">
+        <v>293</v>
       </c>
     </row>
-    <row r="25" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A25" s="11">
         <v>23</v>
       </c>
@@ -19065,10 +19252,10 @@
         <v>86</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>248</v>
+        <v>268</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>247</v>
       </c>
       <c r="G25" s="14">
         <v>89.7</v>
@@ -19799,10 +19986,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ25" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
+      </c>
+      <c r="IK25" s="3" t="s">
+        <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A26" s="11">
         <v>24</v>
       </c>
@@ -19818,8 +20008,8 @@
       <c r="E26" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F26" s="28" t="s">
-        <v>249</v>
+      <c r="F26" s="27" t="s">
+        <v>248</v>
       </c>
       <c r="G26" s="14">
         <v>80</v>
@@ -20549,11 +20739,14 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ26" s="25" t="s">
-        <v>211</v>
+      <c r="IJ26" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="IK26" s="3" t="s">
+        <v>294</v>
       </c>
     </row>
-    <row r="27" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A27" s="11">
         <v>25</v>
       </c>
@@ -20569,8 +20762,8 @@
       <c r="E27" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="F27" s="28" t="s">
-        <v>250</v>
+      <c r="F27" s="27" t="s">
+        <v>249</v>
       </c>
       <c r="G27" s="14">
         <v>81</v>
@@ -21300,11 +21493,14 @@
         <f t="shared" si="16"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="IJ27" s="25" t="s">
-        <v>212</v>
+      <c r="IJ27" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="IK27" s="3" t="s">
+        <v>295</v>
       </c>
     </row>
-    <row r="28" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A28" s="11">
         <v>26</v>
       </c>
@@ -21320,8 +21516,8 @@
       <c r="E28" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="28" t="s">
-        <v>251</v>
+      <c r="F28" s="27" t="s">
+        <v>250</v>
       </c>
       <c r="G28" s="14">
         <v>80</v>
@@ -22051,11 +22247,14 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ28" s="25" t="s">
-        <v>213</v>
+      <c r="IJ28" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="IK28" s="3" t="s">
+        <v>296</v>
       </c>
     </row>
-    <row r="29" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A29" s="11">
         <v>27</v>
       </c>
@@ -22071,8 +22270,8 @@
       <c r="E29" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F29" s="28" t="s">
-        <v>252</v>
+      <c r="F29" s="27" t="s">
+        <v>251</v>
       </c>
       <c r="G29" s="14">
         <v>82.6</v>
@@ -22803,10 +23002,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ29" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+      <c r="IK29" s="3" t="s">
+        <v>297</v>
       </c>
     </row>
-    <row r="30" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A30" s="11">
         <v>28</v>
       </c>
@@ -22822,8 +23024,8 @@
       <c r="E30" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="F30" s="28" t="s">
-        <v>253</v>
+      <c r="F30" s="27" t="s">
+        <v>252</v>
       </c>
       <c r="G30" s="14">
         <v>80</v>
@@ -23554,14 +23756,17 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ30" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
+      </c>
+      <c r="IK30" s="3" t="s">
+        <v>298</v>
       </c>
     </row>
-    <row r="31" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>29</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C31" s="8">
@@ -23573,8 +23778,8 @@
       <c r="E31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="F31" s="28" t="s">
-        <v>254</v>
+      <c r="F31" s="27" t="s">
+        <v>253</v>
       </c>
       <c r="G31" s="14">
         <v>79</v>
@@ -24305,8 +24510,9 @@
         <v>Excellent</v>
       </c>
       <c r="IJ31" s="3"/>
+      <c r="IK31" s="3"/>
     </row>
-    <row r="32" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>30</v>
       </c>
@@ -24322,8 +24528,8 @@
       <c r="E32" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="28" t="s">
-        <v>255</v>
+      <c r="F32" s="27" t="s">
+        <v>254</v>
       </c>
       <c r="G32" s="14">
         <v>79.3</v>
@@ -25054,10 +25260,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ32" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
+      </c>
+      <c r="IK32" s="3" t="s">
+        <v>299</v>
       </c>
     </row>
-    <row r="33" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>31</v>
       </c>
@@ -25073,8 +25282,8 @@
       <c r="E33" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="F33" s="28" t="s">
-        <v>256</v>
+      <c r="F33" s="27" t="s">
+        <v>255</v>
       </c>
       <c r="G33" s="14">
         <v>84.55</v>
@@ -25805,10 +26014,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ33" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
+      </c>
+      <c r="IK33" s="3" t="s">
+        <v>300</v>
       </c>
     </row>
-    <row r="34" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>32</v>
       </c>
@@ -25824,8 +26036,8 @@
       <c r="E34" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="F34" s="28" t="s">
-        <v>257</v>
+      <c r="F34" s="27" t="s">
+        <v>256</v>
       </c>
       <c r="G34" s="14">
         <v>72.600000000000009</v>
@@ -26556,10 +26768,13 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ34" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
+      </c>
+      <c r="IK34" s="3" t="s">
+        <v>301</v>
       </c>
     </row>
-    <row r="35" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>33</v>
       </c>
@@ -26575,8 +26790,8 @@
       <c r="E35" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="F35" s="28" t="s">
-        <v>258</v>
+      <c r="F35" s="27" t="s">
+        <v>257</v>
       </c>
       <c r="G35" s="14">
         <v>91.35</v>
@@ -27307,10 +27522,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ35" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
+      </c>
+      <c r="IK35" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
-    <row r="36" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>34</v>
       </c>
@@ -27326,8 +27544,8 @@
       <c r="E36" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="F36" s="28" t="s">
-        <v>259</v>
+      <c r="F36" s="27" t="s">
+        <v>258</v>
       </c>
       <c r="G36" s="14">
         <v>82.55</v>
@@ -28057,11 +28275,14 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ36" s="25" t="s">
-        <v>268</v>
+      <c r="IJ36" s="37" t="s">
+        <v>267</v>
+      </c>
+      <c r="IK36" s="3" t="s">
+        <v>303</v>
       </c>
     </row>
-    <row r="37" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>35</v>
       </c>
@@ -28077,8 +28298,8 @@
       <c r="E37" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="F37" s="28" t="s">
-        <v>260</v>
+      <c r="F37" s="27" t="s">
+        <v>259</v>
       </c>
       <c r="G37" s="14">
         <v>80.95</v>
@@ -28809,10 +29030,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ37" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
+      </c>
+      <c r="IK37" s="3" t="s">
+        <v>304</v>
       </c>
     </row>
-    <row r="38" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A38" s="11">
         <v>36</v>
       </c>
@@ -28828,8 +29052,8 @@
       <c r="E38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="F38" s="28" t="s">
-        <v>261</v>
+      <c r="F38" s="27" t="s">
+        <v>260</v>
       </c>
       <c r="G38" s="14">
         <v>84.4</v>
@@ -29560,10 +29784,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ38" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
+      </c>
+      <c r="IK38" s="3" t="s">
+        <v>305</v>
       </c>
     </row>
-    <row r="39" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A39" s="11">
         <v>37</v>
       </c>
@@ -29579,8 +29806,8 @@
       <c r="E39" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="28" t="s">
-        <v>262</v>
+      <c r="F39" s="27" t="s">
+        <v>261</v>
       </c>
       <c r="G39" s="14">
         <v>87.700000000000017</v>
@@ -30311,10 +30538,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ39" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="IK39" s="3" t="s">
+        <v>306</v>
       </c>
     </row>
-    <row r="40" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A40" s="11">
         <v>38</v>
       </c>
@@ -30330,8 +30560,8 @@
       <c r="E40" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="F40" s="28" t="s">
-        <v>263</v>
+      <c r="F40" s="27" t="s">
+        <v>262</v>
       </c>
       <c r="G40" s="14">
         <v>86.75</v>
@@ -31062,10 +31292,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ40" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
+      </c>
+      <c r="IK40" s="3" t="s">
+        <v>307</v>
       </c>
     </row>
-    <row r="41" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A41" s="11">
         <v>39</v>
       </c>
@@ -31081,8 +31314,8 @@
       <c r="E41" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="F41" s="28" t="s">
-        <v>264</v>
+      <c r="F41" s="27" t="s">
+        <v>263</v>
       </c>
       <c r="G41" s="14">
         <v>85.600000000000009</v>
@@ -31813,10 +32046,13 @@
         <v>Excellent</v>
       </c>
       <c r="IJ41" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
+      </c>
+      <c r="IK41" s="3" t="s">
+        <v>308</v>
       </c>
     </row>
-    <row r="42" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A42" s="11">
         <v>40</v>
       </c>
@@ -31832,8 +32068,8 @@
       <c r="E42" s="7" t="s">
         <v>111</v>
       </c>
-      <c r="F42" s="28" t="s">
-        <v>265</v>
+      <c r="F42" s="27" t="s">
+        <v>264</v>
       </c>
       <c r="G42" s="14">
         <v>86.300000000000011</v>
@@ -32564,14 +32800,17 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ42" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
+      </c>
+      <c r="IK42" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
-    <row r="43" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A43" s="11">
         <v>41</v>
       </c>
-      <c r="B43" s="27" t="s">
+      <c r="B43" s="26" t="s">
         <v>40</v>
       </c>
       <c r="C43" s="8">
@@ -32583,8 +32822,8 @@
       <c r="E43" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="28" t="s">
-        <v>266</v>
+      <c r="F43" s="27" t="s">
+        <v>265</v>
       </c>
       <c r="G43" s="14">
         <v>75.149999999999991</v>
@@ -33315,70 +33554,17 @@
         <v>Highly Satisfactory</v>
       </c>
       <c r="IJ43" s="3"/>
+      <c r="IK43" s="3"/>
     </row>
-    <row r="44" spans="1:244" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:245" x14ac:dyDescent="0.25">
       <c r="B44" s="12"/>
       <c r="G44" s="9"/>
       <c r="HI44" s="19"/>
       <c r="HN44" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="68">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="BJ1:BN1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="BE1:BI1"/>
-    <mergeCell ref="DR1:DV1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BT1:BX1"/>
-    <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="CI1:CM1"/>
-    <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="FZ1:GD1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EB1:EF1"/>
-    <mergeCell ref="EG1:EK1"/>
-    <mergeCell ref="EL1:EP1"/>
-    <mergeCell ref="EQ1:EU1"/>
-    <mergeCell ref="EV1:EZ1"/>
-    <mergeCell ref="FA1:FE1"/>
-    <mergeCell ref="FF1:FJ1"/>
-    <mergeCell ref="FK1:FO1"/>
-    <mergeCell ref="FP1:FT1"/>
-    <mergeCell ref="FU1:FY1"/>
-    <mergeCell ref="HI1:HM1"/>
-    <mergeCell ref="HN1:HR1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="GJ1:GN1"/>
-    <mergeCell ref="GO1:GS1"/>
-    <mergeCell ref="GT1:GX1"/>
-    <mergeCell ref="GY1:HC1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="HS1:HS2"/>
-    <mergeCell ref="HU1:HU2"/>
-    <mergeCell ref="HW1:HW2"/>
-    <mergeCell ref="HY1:HY2"/>
-    <mergeCell ref="IA1:IA2"/>
+  <mergeCells count="69">
+    <mergeCell ref="IK1:IK2"/>
     <mergeCell ref="II1:II2"/>
     <mergeCell ref="IJ1:IJ2"/>
     <mergeCell ref="HT1:HT2"/>
@@ -33392,6 +33578,61 @@
     <mergeCell ref="IF1:IF2"/>
     <mergeCell ref="IE1:IE2"/>
     <mergeCell ref="IH1:IH2"/>
+    <mergeCell ref="HS1:HS2"/>
+    <mergeCell ref="HU1:HU2"/>
+    <mergeCell ref="HW1:HW2"/>
+    <mergeCell ref="HY1:HY2"/>
+    <mergeCell ref="IA1:IA2"/>
+    <mergeCell ref="HI1:HM1"/>
+    <mergeCell ref="HN1:HR1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="GJ1:GN1"/>
+    <mergeCell ref="GO1:GS1"/>
+    <mergeCell ref="GT1:GX1"/>
+    <mergeCell ref="GY1:HC1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="FZ1:GD1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EB1:EF1"/>
+    <mergeCell ref="EG1:EK1"/>
+    <mergeCell ref="EL1:EP1"/>
+    <mergeCell ref="EQ1:EU1"/>
+    <mergeCell ref="EV1:EZ1"/>
+    <mergeCell ref="FA1:FE1"/>
+    <mergeCell ref="FF1:FJ1"/>
+    <mergeCell ref="FK1:FO1"/>
+    <mergeCell ref="FP1:FT1"/>
+    <mergeCell ref="FU1:FY1"/>
+    <mergeCell ref="DR1:DV1"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="BT1:BX1"/>
+    <mergeCell ref="BY1:CC1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="CI1:CM1"/>
+    <mergeCell ref="CN1:CR1"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DH1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BE1:BI1"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
penambahan judul,no transkip, judul inggris dll
</commit_message>
<xml_diff>
--- a/D3 Keperawatan/Transkip Nilai D3 Kep.xlsx
+++ b/D3 Keperawatan/Transkip Nilai D3 Kep.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nando\Documents\Stikes\Transkip Nilai 2025\D3 Keperawatan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB9F06DD-347F-4C62-8E13-E66F29712585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF38C33A-4E1D-4231-AD88-7CBB3D26DAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22668FF5-9BBF-4EB6-990E-3DE3502F0C5B}"/>
   </bookViews>
@@ -1142,7 +1142,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1211,11 +1211,23 @@
     <xf numFmtId="49" fontId="4" fillId="3" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1223,25 +1235,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Good 2" xfId="4" xr:uid="{9E58217C-29C0-4F6B-BCCA-FBD9D11D267D}"/>
@@ -1562,11 +1561,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2967CDF3-E1DE-4ED6-83C3-5F7B380BED6A}">
   <dimension ref="A1:IK44"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="3" ySplit="2" topLeftCell="IF30" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="3" ySplit="2" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="IK42" sqref="IK42"/>
+      <selection pane="bottomRight" activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1580,148 +1579,148 @@
     <col min="241" max="241" width="13" bestFit="1" customWidth="1"/>
     <col min="242" max="242" width="27.5703125" customWidth="1"/>
     <col min="243" max="243" width="24.28515625" style="1" customWidth="1"/>
-    <col min="244" max="244" width="18.85546875" customWidth="1"/>
-    <col min="245" max="245" width="17.5703125" customWidth="1"/>
+    <col min="244" max="244" width="185.7109375" bestFit="1" customWidth="1"/>
+    <col min="245" max="245" width="190.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:245" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="28" t="s">
+      <c r="C1" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="28" t="s">
+      <c r="F1" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31" t="s">
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
-      <c r="Q1" s="31" t="s">
+      <c r="M1" s="35"/>
+      <c r="N1" s="35"/>
+      <c r="O1" s="35"/>
+      <c r="P1" s="35"/>
+      <c r="Q1" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="R1" s="31"/>
-      <c r="S1" s="31"/>
-      <c r="T1" s="31"/>
-      <c r="U1" s="31"/>
-      <c r="V1" s="31" t="s">
+      <c r="R1" s="35"/>
+      <c r="S1" s="35"/>
+      <c r="T1" s="35"/>
+      <c r="U1" s="35"/>
+      <c r="V1" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="W1" s="31"/>
-      <c r="X1" s="31"/>
-      <c r="Y1" s="31"/>
-      <c r="Z1" s="31"/>
-      <c r="AA1" s="31" t="s">
+      <c r="W1" s="35"/>
+      <c r="X1" s="35"/>
+      <c r="Y1" s="35"/>
+      <c r="Z1" s="35"/>
+      <c r="AA1" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="AB1" s="31"/>
-      <c r="AC1" s="31"/>
-      <c r="AD1" s="31"/>
-      <c r="AE1" s="31"/>
-      <c r="AF1" s="31" t="s">
+      <c r="AB1" s="35"/>
+      <c r="AC1" s="35"/>
+      <c r="AD1" s="35"/>
+      <c r="AE1" s="35"/>
+      <c r="AF1" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="AG1" s="31"/>
-      <c r="AH1" s="31"/>
-      <c r="AI1" s="31"/>
-      <c r="AJ1" s="31"/>
-      <c r="AK1" s="31" t="s">
+      <c r="AG1" s="35"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="35"/>
+      <c r="AJ1" s="35"/>
+      <c r="AK1" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="AL1" s="31"/>
-      <c r="AM1" s="31"/>
-      <c r="AN1" s="31"/>
-      <c r="AO1" s="31"/>
-      <c r="AP1" s="31" t="s">
+      <c r="AL1" s="35"/>
+      <c r="AM1" s="35"/>
+      <c r="AN1" s="35"/>
+      <c r="AO1" s="35"/>
+      <c r="AP1" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="AQ1" s="31"/>
-      <c r="AR1" s="31"/>
-      <c r="AS1" s="31"/>
-      <c r="AT1" s="31"/>
-      <c r="AU1" s="31" t="s">
+      <c r="AQ1" s="35"/>
+      <c r="AR1" s="35"/>
+      <c r="AS1" s="35"/>
+      <c r="AT1" s="35"/>
+      <c r="AU1" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="AV1" s="31"/>
-      <c r="AW1" s="31"/>
-      <c r="AX1" s="31"/>
-      <c r="AY1" s="31"/>
-      <c r="AZ1" s="30" t="s">
+      <c r="AV1" s="35"/>
+      <c r="AW1" s="35"/>
+      <c r="AX1" s="35"/>
+      <c r="AY1" s="35"/>
+      <c r="AZ1" s="34" t="s">
         <v>128</v>
       </c>
-      <c r="BA1" s="30"/>
-      <c r="BB1" s="30"/>
-      <c r="BC1" s="30"/>
-      <c r="BD1" s="30"/>
-      <c r="BE1" s="30" t="s">
+      <c r="BA1" s="34"/>
+      <c r="BB1" s="34"/>
+      <c r="BC1" s="34"/>
+      <c r="BD1" s="34"/>
+      <c r="BE1" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="BF1" s="30"/>
-      <c r="BG1" s="30"/>
-      <c r="BH1" s="30"/>
-      <c r="BI1" s="30"/>
-      <c r="BJ1" s="30" t="s">
+      <c r="BF1" s="34"/>
+      <c r="BG1" s="34"/>
+      <c r="BH1" s="34"/>
+      <c r="BI1" s="34"/>
+      <c r="BJ1" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="BK1" s="30"/>
-      <c r="BL1" s="30"/>
-      <c r="BM1" s="30"/>
-      <c r="BN1" s="30"/>
-      <c r="BO1" s="30" t="s">
+      <c r="BK1" s="34"/>
+      <c r="BL1" s="34"/>
+      <c r="BM1" s="34"/>
+      <c r="BN1" s="34"/>
+      <c r="BO1" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="BP1" s="30"/>
-      <c r="BQ1" s="30"/>
-      <c r="BR1" s="30"/>
-      <c r="BS1" s="30"/>
-      <c r="BT1" s="30" t="s">
+      <c r="BP1" s="34"/>
+      <c r="BQ1" s="34"/>
+      <c r="BR1" s="34"/>
+      <c r="BS1" s="34"/>
+      <c r="BT1" s="34" t="s">
         <v>132</v>
       </c>
-      <c r="BU1" s="30"/>
-      <c r="BV1" s="30"/>
-      <c r="BW1" s="30"/>
-      <c r="BX1" s="30"/>
-      <c r="BY1" s="30" t="s">
+      <c r="BU1" s="34"/>
+      <c r="BV1" s="34"/>
+      <c r="BW1" s="34"/>
+      <c r="BX1" s="34"/>
+      <c r="BY1" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="BZ1" s="30"/>
-      <c r="CA1" s="30"/>
-      <c r="CB1" s="30"/>
-      <c r="CC1" s="30"/>
-      <c r="CD1" s="30" t="s">
+      <c r="BZ1" s="34"/>
+      <c r="CA1" s="34"/>
+      <c r="CB1" s="34"/>
+      <c r="CC1" s="34"/>
+      <c r="CD1" s="34" t="s">
         <v>134</v>
       </c>
-      <c r="CE1" s="30"/>
-      <c r="CF1" s="30"/>
-      <c r="CG1" s="30"/>
-      <c r="CH1" s="30"/>
-      <c r="CI1" s="30" t="s">
+      <c r="CE1" s="34"/>
+      <c r="CF1" s="34"/>
+      <c r="CG1" s="34"/>
+      <c r="CH1" s="34"/>
+      <c r="CI1" s="34" t="s">
         <v>135</v>
       </c>
-      <c r="CJ1" s="30"/>
-      <c r="CK1" s="30"/>
-      <c r="CL1" s="30"/>
-      <c r="CM1" s="30"/>
+      <c r="CJ1" s="34"/>
+      <c r="CK1" s="34"/>
+      <c r="CL1" s="34"/>
+      <c r="CM1" s="34"/>
       <c r="CN1" s="32" t="s">
         <v>138</v>
       </c>
@@ -1778,204 +1777,204 @@
       <c r="DY1" s="32"/>
       <c r="DZ1" s="32"/>
       <c r="EA1" s="32"/>
-      <c r="EB1" s="34" t="s">
+      <c r="EB1" s="33" t="s">
         <v>146</v>
       </c>
-      <c r="EC1" s="34"/>
-      <c r="ED1" s="34"/>
-      <c r="EE1" s="34"/>
-      <c r="EF1" s="34"/>
-      <c r="EG1" s="34" t="s">
+      <c r="EC1" s="33"/>
+      <c r="ED1" s="33"/>
+      <c r="EE1" s="33"/>
+      <c r="EF1" s="33"/>
+      <c r="EG1" s="33" t="s">
         <v>147</v>
       </c>
-      <c r="EH1" s="34"/>
-      <c r="EI1" s="34"/>
-      <c r="EJ1" s="34"/>
-      <c r="EK1" s="34"/>
-      <c r="EL1" s="34" t="s">
+      <c r="EH1" s="33"/>
+      <c r="EI1" s="33"/>
+      <c r="EJ1" s="33"/>
+      <c r="EK1" s="33"/>
+      <c r="EL1" s="33" t="s">
         <v>148</v>
       </c>
-      <c r="EM1" s="34"/>
-      <c r="EN1" s="34"/>
-      <c r="EO1" s="34"/>
-      <c r="EP1" s="34"/>
-      <c r="EQ1" s="34" t="s">
+      <c r="EM1" s="33"/>
+      <c r="EN1" s="33"/>
+      <c r="EO1" s="33"/>
+      <c r="EP1" s="33"/>
+      <c r="EQ1" s="33" t="s">
         <v>149</v>
       </c>
-      <c r="ER1" s="34"/>
-      <c r="ES1" s="34"/>
-      <c r="ET1" s="34"/>
-      <c r="EU1" s="34"/>
-      <c r="EV1" s="34" t="s">
+      <c r="ER1" s="33"/>
+      <c r="ES1" s="33"/>
+      <c r="ET1" s="33"/>
+      <c r="EU1" s="33"/>
+      <c r="EV1" s="33" t="s">
         <v>150</v>
       </c>
-      <c r="EW1" s="34"/>
-      <c r="EX1" s="34"/>
-      <c r="EY1" s="34"/>
-      <c r="EZ1" s="34"/>
-      <c r="FA1" s="34" t="s">
+      <c r="EW1" s="33"/>
+      <c r="EX1" s="33"/>
+      <c r="EY1" s="33"/>
+      <c r="EZ1" s="33"/>
+      <c r="FA1" s="33" t="s">
         <v>151</v>
       </c>
-      <c r="FB1" s="34"/>
-      <c r="FC1" s="34"/>
-      <c r="FD1" s="34"/>
-      <c r="FE1" s="34"/>
-      <c r="FF1" s="34" t="s">
+      <c r="FB1" s="33"/>
+      <c r="FC1" s="33"/>
+      <c r="FD1" s="33"/>
+      <c r="FE1" s="33"/>
+      <c r="FF1" s="33" t="s">
         <v>152</v>
       </c>
-      <c r="FG1" s="34"/>
-      <c r="FH1" s="34"/>
-      <c r="FI1" s="34"/>
-      <c r="FJ1" s="34"/>
-      <c r="FK1" s="34" t="s">
+      <c r="FG1" s="33"/>
+      <c r="FH1" s="33"/>
+      <c r="FI1" s="33"/>
+      <c r="FJ1" s="33"/>
+      <c r="FK1" s="33" t="s">
         <v>153</v>
       </c>
-      <c r="FL1" s="34"/>
-      <c r="FM1" s="34"/>
-      <c r="FN1" s="34"/>
-      <c r="FO1" s="34"/>
-      <c r="FP1" s="33" t="s">
+      <c r="FL1" s="33"/>
+      <c r="FM1" s="33"/>
+      <c r="FN1" s="33"/>
+      <c r="FO1" s="33"/>
+      <c r="FP1" s="31" t="s">
         <v>155</v>
       </c>
-      <c r="FQ1" s="33"/>
-      <c r="FR1" s="33"/>
-      <c r="FS1" s="33"/>
-      <c r="FT1" s="33"/>
-      <c r="FU1" s="33" t="s">
+      <c r="FQ1" s="31"/>
+      <c r="FR1" s="31"/>
+      <c r="FS1" s="31"/>
+      <c r="FT1" s="31"/>
+      <c r="FU1" s="31" t="s">
         <v>156</v>
       </c>
-      <c r="FV1" s="33"/>
-      <c r="FW1" s="33"/>
-      <c r="FX1" s="33"/>
-      <c r="FY1" s="33"/>
-      <c r="FZ1" s="33" t="s">
+      <c r="FV1" s="31"/>
+      <c r="FW1" s="31"/>
+      <c r="FX1" s="31"/>
+      <c r="FY1" s="31"/>
+      <c r="FZ1" s="31" t="s">
         <v>157</v>
       </c>
-      <c r="GA1" s="33"/>
-      <c r="GB1" s="33"/>
-      <c r="GC1" s="33"/>
-      <c r="GD1" s="33"/>
-      <c r="GE1" s="33" t="s">
+      <c r="GA1" s="31"/>
+      <c r="GB1" s="31"/>
+      <c r="GC1" s="31"/>
+      <c r="GD1" s="31"/>
+      <c r="GE1" s="31" t="s">
         <v>158</v>
       </c>
-      <c r="GF1" s="33"/>
-      <c r="GG1" s="33"/>
-      <c r="GH1" s="33"/>
-      <c r="GI1" s="33"/>
-      <c r="GJ1" s="33" t="s">
+      <c r="GF1" s="31"/>
+      <c r="GG1" s="31"/>
+      <c r="GH1" s="31"/>
+      <c r="GI1" s="31"/>
+      <c r="GJ1" s="31" t="s">
         <v>159</v>
       </c>
-      <c r="GK1" s="33"/>
-      <c r="GL1" s="33"/>
-      <c r="GM1" s="33"/>
-      <c r="GN1" s="33"/>
-      <c r="GO1" s="33" t="s">
+      <c r="GK1" s="31"/>
+      <c r="GL1" s="31"/>
+      <c r="GM1" s="31"/>
+      <c r="GN1" s="31"/>
+      <c r="GO1" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="GP1" s="33"/>
-      <c r="GQ1" s="33"/>
-      <c r="GR1" s="33"/>
-      <c r="GS1" s="33"/>
-      <c r="GT1" s="33" t="s">
+      <c r="GP1" s="31"/>
+      <c r="GQ1" s="31"/>
+      <c r="GR1" s="31"/>
+      <c r="GS1" s="31"/>
+      <c r="GT1" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="GU1" s="33"/>
-      <c r="GV1" s="33"/>
-      <c r="GW1" s="33"/>
-      <c r="GX1" s="33"/>
-      <c r="GY1" s="33" t="s">
+      <c r="GU1" s="31"/>
+      <c r="GV1" s="31"/>
+      <c r="GW1" s="31"/>
+      <c r="GX1" s="31"/>
+      <c r="GY1" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="GZ1" s="33"/>
-      <c r="HA1" s="33"/>
-      <c r="HB1" s="33"/>
-      <c r="HC1" s="33"/>
-      <c r="HD1" s="33" t="s">
+      <c r="GZ1" s="31"/>
+      <c r="HA1" s="31"/>
+      <c r="HB1" s="31"/>
+      <c r="HC1" s="31"/>
+      <c r="HD1" s="31" t="s">
         <v>163</v>
       </c>
-      <c r="HE1" s="33"/>
-      <c r="HF1" s="33"/>
-      <c r="HG1" s="33"/>
-      <c r="HH1" s="33"/>
-      <c r="HI1" s="35" t="s">
+      <c r="HE1" s="31"/>
+      <c r="HF1" s="31"/>
+      <c r="HG1" s="31"/>
+      <c r="HH1" s="31"/>
+      <c r="HI1" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="HJ1" s="35"/>
-      <c r="HK1" s="35"/>
-      <c r="HL1" s="35"/>
-      <c r="HM1" s="35"/>
-      <c r="HN1" s="35" t="s">
+      <c r="HJ1" s="30"/>
+      <c r="HK1" s="30"/>
+      <c r="HL1" s="30"/>
+      <c r="HM1" s="30"/>
+      <c r="HN1" s="30" t="s">
         <v>165</v>
       </c>
-      <c r="HO1" s="35"/>
-      <c r="HP1" s="35"/>
-      <c r="HQ1" s="35"/>
-      <c r="HR1" s="35"/>
-      <c r="HS1" s="36" t="s">
+      <c r="HO1" s="30"/>
+      <c r="HP1" s="30"/>
+      <c r="HQ1" s="30"/>
+      <c r="HR1" s="30"/>
+      <c r="HS1" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="HT1" s="36" t="s">
+      <c r="HT1" s="29" t="s">
         <v>178</v>
       </c>
-      <c r="HU1" s="36" t="s">
+      <c r="HU1" s="29" t="s">
         <v>180</v>
       </c>
-      <c r="HV1" s="36" t="s">
+      <c r="HV1" s="29" t="s">
         <v>179</v>
       </c>
-      <c r="HW1" s="36" t="s">
+      <c r="HW1" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="HX1" s="36" t="s">
+      <c r="HX1" s="29" t="s">
         <v>181</v>
       </c>
-      <c r="HY1" s="36" t="s">
+      <c r="HY1" s="29" t="s">
         <v>186</v>
       </c>
-      <c r="HZ1" s="36" t="s">
+      <c r="HZ1" s="29" t="s">
         <v>182</v>
       </c>
-      <c r="IA1" s="36" t="s">
+      <c r="IA1" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="IB1" s="36" t="s">
+      <c r="IB1" s="29" t="s">
         <v>183</v>
       </c>
-      <c r="IC1" s="36" t="s">
+      <c r="IC1" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="ID1" s="36" t="s">
+      <c r="ID1" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="IE1" s="36" t="s">
+      <c r="IE1" s="29" t="s">
         <v>172</v>
       </c>
-      <c r="IF1" s="36" t="s">
+      <c r="IF1" s="29" t="s">
         <v>173</v>
       </c>
-      <c r="IG1" s="36" t="s">
+      <c r="IG1" s="29" t="s">
         <v>189</v>
       </c>
-      <c r="IH1" s="36" t="s">
+      <c r="IH1" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="II1" s="36" t="s">
+      <c r="II1" s="29" t="s">
         <v>175</v>
       </c>
-      <c r="IJ1" s="36" t="s">
+      <c r="IJ1" s="29" t="s">
         <v>176</v>
       </c>
-      <c r="IK1" s="36" t="s">
+      <c r="IK1" s="29" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="2" spans="1:245" x14ac:dyDescent="0.25">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="28"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="36"/>
       <c r="G2" s="10" t="s">
         <v>44</v>
       </c>
@@ -2636,25 +2635,25 @@
       <c r="HR2" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="HS2" s="36"/>
-      <c r="HT2" s="36"/>
-      <c r="HU2" s="36"/>
-      <c r="HV2" s="36"/>
-      <c r="HW2" s="36"/>
-      <c r="HX2" s="36"/>
-      <c r="HY2" s="36"/>
-      <c r="HZ2" s="36"/>
-      <c r="IA2" s="36"/>
-      <c r="IB2" s="36"/>
-      <c r="IC2" s="36"/>
-      <c r="ID2" s="36"/>
-      <c r="IE2" s="36"/>
-      <c r="IF2" s="36"/>
-      <c r="IG2" s="36"/>
-      <c r="IH2" s="36"/>
-      <c r="II2" s="36"/>
-      <c r="IJ2" s="36"/>
-      <c r="IK2" s="36"/>
+      <c r="HS2" s="29"/>
+      <c r="HT2" s="29"/>
+      <c r="HU2" s="29"/>
+      <c r="HV2" s="29"/>
+      <c r="HW2" s="29"/>
+      <c r="HX2" s="29"/>
+      <c r="HY2" s="29"/>
+      <c r="HZ2" s="29"/>
+      <c r="IA2" s="29"/>
+      <c r="IB2" s="29"/>
+      <c r="IC2" s="29"/>
+      <c r="ID2" s="29"/>
+      <c r="IE2" s="29"/>
+      <c r="IF2" s="29"/>
+      <c r="IG2" s="29"/>
+      <c r="IH2" s="29"/>
+      <c r="II2" s="29"/>
+      <c r="IJ2" s="29"/>
+      <c r="IK2" s="29"/>
     </row>
     <row r="3" spans="1:245" x14ac:dyDescent="0.25">
       <c r="A3" s="11">
@@ -3406,7 +3405,7 @@
       <c r="IJ3" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="IK3" s="38" t="s">
+      <c r="IK3" s="3" t="s">
         <v>271</v>
       </c>
     </row>
@@ -13203,7 +13202,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ16" s="37" t="s">
+      <c r="IJ16" s="28" t="s">
         <v>201</v>
       </c>
       <c r="IK16" s="3" t="s">
@@ -20739,7 +20738,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ26" s="37" t="s">
+      <c r="IJ26" s="28" t="s">
         <v>210</v>
       </c>
       <c r="IK26" s="3" t="s">
@@ -21493,7 +21492,7 @@
         <f t="shared" si="16"/>
         <v>Highly Satisfactory</v>
       </c>
-      <c r="IJ27" s="37" t="s">
+      <c r="IJ27" s="28" t="s">
         <v>211</v>
       </c>
       <c r="IK27" s="3" t="s">
@@ -22247,7 +22246,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ28" s="37" t="s">
+      <c r="IJ28" s="28" t="s">
         <v>212</v>
       </c>
       <c r="IK28" s="3" t="s">
@@ -28275,7 +28274,7 @@
         <f t="shared" si="16"/>
         <v>Excellent</v>
       </c>
-      <c r="IJ36" s="37" t="s">
+      <c r="IJ36" s="28" t="s">
         <v>267</v>
       </c>
       <c r="IK36" s="3" t="s">
@@ -33564,6 +33563,61 @@
     </row>
   </sheetData>
   <mergeCells count="69">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BE1:BI1"/>
+    <mergeCell ref="DR1:DV1"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="BT1:BX1"/>
+    <mergeCell ref="BY1:CC1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="CI1:CM1"/>
+    <mergeCell ref="CN1:CR1"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
+    <mergeCell ref="DH1:DL1"/>
+    <mergeCell ref="DM1:DQ1"/>
+    <mergeCell ref="FZ1:GD1"/>
+    <mergeCell ref="DW1:EA1"/>
+    <mergeCell ref="EB1:EF1"/>
+    <mergeCell ref="EG1:EK1"/>
+    <mergeCell ref="EL1:EP1"/>
+    <mergeCell ref="EQ1:EU1"/>
+    <mergeCell ref="EV1:EZ1"/>
+    <mergeCell ref="FA1:FE1"/>
+    <mergeCell ref="FF1:FJ1"/>
+    <mergeCell ref="FK1:FO1"/>
+    <mergeCell ref="FP1:FT1"/>
+    <mergeCell ref="FU1:FY1"/>
+    <mergeCell ref="HI1:HM1"/>
+    <mergeCell ref="HN1:HR1"/>
+    <mergeCell ref="GE1:GI1"/>
+    <mergeCell ref="GJ1:GN1"/>
+    <mergeCell ref="GO1:GS1"/>
+    <mergeCell ref="GT1:GX1"/>
+    <mergeCell ref="GY1:HC1"/>
+    <mergeCell ref="HD1:HH1"/>
+    <mergeCell ref="HS1:HS2"/>
+    <mergeCell ref="HU1:HU2"/>
+    <mergeCell ref="HW1:HW2"/>
+    <mergeCell ref="HY1:HY2"/>
+    <mergeCell ref="IA1:IA2"/>
     <mergeCell ref="IK1:IK2"/>
     <mergeCell ref="II1:II2"/>
     <mergeCell ref="IJ1:IJ2"/>
@@ -33578,61 +33632,6 @@
     <mergeCell ref="IF1:IF2"/>
     <mergeCell ref="IE1:IE2"/>
     <mergeCell ref="IH1:IH2"/>
-    <mergeCell ref="HS1:HS2"/>
-    <mergeCell ref="HU1:HU2"/>
-    <mergeCell ref="HW1:HW2"/>
-    <mergeCell ref="HY1:HY2"/>
-    <mergeCell ref="IA1:IA2"/>
-    <mergeCell ref="HI1:HM1"/>
-    <mergeCell ref="HN1:HR1"/>
-    <mergeCell ref="GE1:GI1"/>
-    <mergeCell ref="GJ1:GN1"/>
-    <mergeCell ref="GO1:GS1"/>
-    <mergeCell ref="GT1:GX1"/>
-    <mergeCell ref="GY1:HC1"/>
-    <mergeCell ref="HD1:HH1"/>
-    <mergeCell ref="FZ1:GD1"/>
-    <mergeCell ref="DW1:EA1"/>
-    <mergeCell ref="EB1:EF1"/>
-    <mergeCell ref="EG1:EK1"/>
-    <mergeCell ref="EL1:EP1"/>
-    <mergeCell ref="EQ1:EU1"/>
-    <mergeCell ref="EV1:EZ1"/>
-    <mergeCell ref="FA1:FE1"/>
-    <mergeCell ref="FF1:FJ1"/>
-    <mergeCell ref="FK1:FO1"/>
-    <mergeCell ref="FP1:FT1"/>
-    <mergeCell ref="FU1:FY1"/>
-    <mergeCell ref="DR1:DV1"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="BT1:BX1"/>
-    <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="CI1:CM1"/>
-    <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="DH1:DL1"/>
-    <mergeCell ref="DM1:DQ1"/>
-    <mergeCell ref="BJ1:BN1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="BE1:BI1"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>